<commit_message>
dlc, kblad, sdcol updated to latest
</commit_message>
<xml_diff>
--- a/models/dev-layout-conn/source/dev-layout-conn.xlsx
+++ b/models/dev-layout-conn/source/dev-layout-conn.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="504">
   <si>
     <t>id</t>
   </si>
@@ -310,6 +310,9 @@
     <t>41,110in223</t>
   </si>
   <si>
+    <t>w-A-S</t>
+  </si>
+  <si>
     <t>Common carotid artery</t>
   </si>
   <si>
@@ -1150,9 +1153,6 @@
     <t>aa-leaf-3</t>
   </si>
   <si>
-    <t>w-A-E</t>
-  </si>
-  <si>
     <t>RespTra</t>
   </si>
   <si>
@@ -1187,6 +1187,9 @@
   </si>
   <si>
     <t>oeso-leaf-6</t>
+  </si>
+  <si>
+    <t>w-O-X</t>
   </si>
   <si>
     <t>IML1-SCG-d</t>
@@ -1604,6 +1607,9 @@
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
@@ -1623,9 +1629,6 @@
     <font>
       <color rgb="FF555555"/>
       <name val="&quot;docs-Helvetica Neue&quot;"/>
-    </font>
-    <font>
-      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF222222"/>
@@ -1760,7 +1763,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1878,13 +1881,16 @@
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1905,129 +1911,129 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -2040,22 +2046,22 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2073,10 +2079,10 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2426,98 +2432,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="B2" s="118" t="s">
         <v>482</v>
+      </c>
+      <c r="B2" s="119" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>483</v>
-      </c>
-      <c r="B3" s="119" t="s">
         <v>484</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="B4" s="120" t="s">
         <v>486</v>
+      </c>
+      <c r="B4" s="121" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>487</v>
-      </c>
-      <c r="B5" s="120" t="s">
         <v>488</v>
+      </c>
+      <c r="B5" s="121" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
-        <v>489</v>
-      </c>
-      <c r="B6" s="120" t="s">
         <v>490</v>
+      </c>
+      <c r="B6" s="121" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
-        <v>491</v>
-      </c>
-      <c r="B7" s="120" t="s">
         <v>492</v>
+      </c>
+      <c r="B7" s="121" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="18" t="s">
-        <v>493</v>
-      </c>
-      <c r="B8" s="120" t="s">
         <v>494</v>
+      </c>
+      <c r="B8" s="121" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="18" t="s">
-        <v>495</v>
-      </c>
-      <c r="B9" s="120" t="s">
         <v>496</v>
+      </c>
+      <c r="B9" s="121" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="B10" s="120" t="s">
         <v>498</v>
+      </c>
+      <c r="B10" s="121" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="18" t="s">
-        <v>499</v>
-      </c>
-      <c r="B11" s="120" t="s">
         <v>500</v>
+      </c>
+      <c r="B11" s="121" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="30" t="s">
-        <v>501</v>
-      </c>
-      <c r="B12" s="121" t="s">
         <v>502</v>
+      </c>
+      <c r="B12" s="122" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
@@ -3315,25 +3321,27 @@
       <c r="P25" s="18"/>
       <c r="Q25" s="21"/>
       <c r="R25" s="18"/>
-      <c r="T25" s="22"/>
+      <c r="T25" s="39" t="s">
+        <v>86</v>
+      </c>
       <c r="U25" s="22"/>
     </row>
     <row r="26">
       <c r="A26" s="15">
         <v>224.0</v>
       </c>
-      <c r="B26" s="39" t="s">
-        <v>86</v>
+      <c r="B26" s="40" t="s">
+        <v>87</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="19"/>
       <c r="F26" s="16"/>
       <c r="G26" s="18"/>
       <c r="I26" s="20" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J26" s="18"/>
       <c r="L26" s="18"/>
@@ -3350,18 +3358,18 @@
       <c r="A27" s="15">
         <v>225.0</v>
       </c>
-      <c r="B27" s="39" t="s">
-        <v>89</v>
+      <c r="B27" s="40" t="s">
+        <v>90</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="19"/>
       <c r="F27" s="16"/>
       <c r="G27" s="18"/>
       <c r="I27" s="20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J27" s="18"/>
       <c r="L27" s="18"/>
@@ -3376,23 +3384,23 @@
     </row>
     <row r="28">
       <c r="A28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="B28" s="39" t="s">
         <v>93</v>
       </c>
+      <c r="B28" s="40" t="s">
+        <v>94</v>
+      </c>
       <c r="C28" s="25" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="19"/>
       <c r="F28" s="16"/>
       <c r="G28" s="18"/>
       <c r="I28" s="20"/>
-      <c r="J28" s="40">
+      <c r="J28" s="41">
         <v>110.0</v>
       </c>
-      <c r="M28" s="41">
+      <c r="M28" s="42">
         <v>254.0</v>
       </c>
       <c r="N28" s="26">
@@ -3407,23 +3415,23 @@
     </row>
     <row r="29">
       <c r="A29" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="39" t="s">
         <v>96</v>
       </c>
+      <c r="B29" s="40" t="s">
+        <v>97</v>
+      </c>
       <c r="C29" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="19"/>
       <c r="F29" s="16"/>
       <c r="G29" s="18"/>
       <c r="I29" s="20"/>
-      <c r="J29" s="40">
+      <c r="J29" s="41">
         <v>110.0</v>
       </c>
-      <c r="M29" s="41">
+      <c r="M29" s="42">
         <v>255.0</v>
       </c>
       <c r="N29" s="26">
@@ -3438,23 +3446,23 @@
     </row>
     <row r="30">
       <c r="A30" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B30" s="39" t="s">
         <v>99</v>
       </c>
+      <c r="B30" s="40" t="s">
+        <v>100</v>
+      </c>
       <c r="C30" s="25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D30" s="18"/>
       <c r="E30" s="19"/>
       <c r="F30" s="16"/>
       <c r="G30" s="18"/>
       <c r="I30" s="20"/>
-      <c r="J30" s="40">
+      <c r="J30" s="41">
         <v>110.0</v>
       </c>
-      <c r="M30" s="41">
+      <c r="M30" s="42">
         <v>256.0</v>
       </c>
       <c r="N30" s="26">
@@ -3471,18 +3479,18 @@
       <c r="A31" s="15">
         <v>226.0</v>
       </c>
-      <c r="B31" s="42" t="s">
-        <v>101</v>
+      <c r="B31" s="43" t="s">
+        <v>102</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D31" s="18"/>
       <c r="E31" s="19"/>
       <c r="F31" s="16"/>
       <c r="G31" s="18"/>
       <c r="I31" s="20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J31" s="18"/>
       <c r="L31" s="18"/>
@@ -3499,18 +3507,18 @@
       <c r="A32" s="15">
         <v>227.0</v>
       </c>
-      <c r="B32" s="42" t="s">
-        <v>104</v>
+      <c r="B32" s="43" t="s">
+        <v>105</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D32" s="18"/>
       <c r="E32" s="19"/>
       <c r="F32" s="16"/>
       <c r="G32" s="18"/>
-      <c r="I32" s="43" t="s">
-        <v>106</v>
+      <c r="I32" s="44" t="s">
+        <v>107</v>
       </c>
       <c r="J32" s="18"/>
       <c r="L32" s="18"/>
@@ -3528,10 +3536,10 @@
         <v>228.0</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D33" s="18"/>
       <c r="E33" s="19"/>
@@ -3540,9 +3548,9 @@
       <c r="I33" s="20"/>
       <c r="J33" s="26"/>
       <c r="M33" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="N33" s="44">
+        <v>110</v>
+      </c>
+      <c r="N33" s="45">
         <v>0.0</v>
       </c>
       <c r="O33" s="18"/>
@@ -3557,17 +3565,17 @@
         <v>229.0</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="C34" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="E34" s="46" t="b">
+      <c r="C34" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="47" t="b">
         <v>1</v>
       </c>
       <c r="G34" s="18"/>
       <c r="I34" s="20" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J34" s="18"/>
       <c r="L34" s="18"/>
@@ -3581,20 +3589,20 @@
       <c r="U34" s="22"/>
     </row>
     <row r="35">
-      <c r="A35" s="47" t="s">
-        <v>113</v>
+      <c r="A35" s="48" t="s">
+        <v>114</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="E35" s="49" t="b">
+        <v>115</v>
+      </c>
+      <c r="C35" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" s="50" t="b">
         <v>1</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="18"/>
@@ -3609,20 +3617,20 @@
       <c r="U35" s="22"/>
     </row>
     <row r="36">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="50" t="b">
+        <v>1</v>
+      </c>
+      <c r="F36" s="51" t="s">
         <v>116</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="C36" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="F36" s="50" t="s">
-        <v>115</v>
       </c>
       <c r="I36" s="20"/>
       <c r="J36" s="18"/>
@@ -3637,20 +3645,20 @@
       <c r="U36" s="22"/>
     </row>
     <row r="37">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="C37" s="48" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" s="49" t="b">
+      <c r="E37" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="F37" s="50" t="s">
-        <v>121</v>
+      <c r="F37" s="51" t="s">
+        <v>122</v>
       </c>
       <c r="I37" s="20"/>
       <c r="J37" s="18"/>
@@ -3665,20 +3673,20 @@
       <c r="U37" s="22"/>
     </row>
     <row r="38">
-      <c r="A38" s="47" t="s">
-        <v>122</v>
+      <c r="A38" s="48" t="s">
+        <v>123</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C38" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="E38" s="49" t="b">
+      <c r="C38" s="49" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="F38" s="50" t="s">
-        <v>115</v>
+      <c r="F38" s="51" t="s">
+        <v>116</v>
       </c>
       <c r="I38" s="20"/>
       <c r="J38" s="18"/>
@@ -3693,20 +3701,20 @@
       <c r="U38" s="22"/>
     </row>
     <row r="39">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B39" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="E39" s="49" t="b">
+      <c r="E39" s="50" t="b">
         <v>1</v>
       </c>
-      <c r="F39" s="50" t="s">
-        <v>121</v>
+      <c r="F39" s="51" t="s">
+        <v>122</v>
       </c>
       <c r="I39" s="20"/>
       <c r="J39" s="18"/>
@@ -3722,23 +3730,23 @@
     </row>
     <row r="40">
       <c r="A40" s="15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" s="45" t="s">
         <v>129</v>
+      </c>
+      <c r="C40" s="46" t="s">
+        <v>130</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="19"/>
       <c r="F40" s="16"/>
       <c r="G40" s="18"/>
       <c r="I40" s="20"/>
-      <c r="J40" s="40">
+      <c r="J40" s="41">
         <v>107.0</v>
       </c>
-      <c r="M40" s="51">
+      <c r="M40" s="52">
         <v>228.0</v>
       </c>
       <c r="N40" s="26">
@@ -3753,23 +3761,23 @@
     </row>
     <row r="41">
       <c r="A41" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="45" t="s">
         <v>132</v>
+      </c>
+      <c r="C41" s="46" t="s">
+        <v>133</v>
       </c>
       <c r="D41" s="18"/>
       <c r="E41" s="19"/>
       <c r="F41" s="16"/>
       <c r="G41" s="18"/>
       <c r="I41" s="20"/>
-      <c r="J41" s="40">
+      <c r="J41" s="41">
         <v>107.0</v>
       </c>
-      <c r="M41" s="40">
+      <c r="M41" s="41">
         <v>201.0</v>
       </c>
       <c r="N41" s="26">
@@ -3786,11 +3794,11 @@
       <c r="A42" s="15">
         <v>230.0</v>
       </c>
-      <c r="B42" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" s="45" t="s">
+      <c r="B42" s="53" t="s">
         <v>134</v>
+      </c>
+      <c r="C42" s="46" t="s">
+        <v>135</v>
       </c>
       <c r="D42" s="18"/>
       <c r="E42" s="19"/>
@@ -3814,11 +3822,11 @@
       <c r="A43" s="15">
         <v>231.0</v>
       </c>
-      <c r="B43" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="C43" s="45" t="s">
+      <c r="B43" s="53" t="s">
         <v>136</v>
+      </c>
+      <c r="C43" s="46" t="s">
+        <v>137</v>
       </c>
       <c r="D43" s="18"/>
       <c r="E43" s="19"/>
@@ -3845,11 +3853,11 @@
       <c r="A44" s="15">
         <v>232.0</v>
       </c>
-      <c r="B44" s="52" t="s">
-        <v>137</v>
-      </c>
-      <c r="C44" s="45" t="s">
+      <c r="B44" s="53" t="s">
         <v>138</v>
+      </c>
+      <c r="C44" s="46" t="s">
+        <v>139</v>
       </c>
       <c r="D44" s="18"/>
       <c r="E44" s="19"/>
@@ -3866,7 +3874,7 @@
       <c r="P44" s="18"/>
       <c r="Q44" s="21"/>
       <c r="R44" s="18"/>
-      <c r="S44" s="30" t="s">
+      <c r="S44" s="3" t="s">
         <v>67</v>
       </c>
       <c r="T44" s="22"/>
@@ -3876,11 +3884,11 @@
       <c r="A45" s="15">
         <v>233.0</v>
       </c>
-      <c r="B45" s="52" t="s">
-        <v>139</v>
-      </c>
-      <c r="C45" s="45" t="s">
+      <c r="B45" s="53" t="s">
         <v>140</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>141</v>
       </c>
       <c r="D45" s="18"/>
       <c r="E45" s="19"/>
@@ -3893,11 +3901,10 @@
       <c r="L45" s="18"/>
       <c r="M45" s="16"/>
       <c r="N45" s="18"/>
-      <c r="O45" s="18"/>
       <c r="P45" s="18"/>
       <c r="Q45" s="21"/>
       <c r="R45" s="18"/>
-      <c r="S45" s="30" t="s">
+      <c r="S45" s="3" t="s">
         <v>70</v>
       </c>
       <c r="T45" s="22"/>
@@ -3907,20 +3914,20 @@
       <c r="A46" s="15">
         <v>234.0</v>
       </c>
-      <c r="B46" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="45" t="s">
+      <c r="B46" s="53" t="s">
         <v>142</v>
+      </c>
+      <c r="C46" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="D46" s="18"/>
       <c r="E46" s="19"/>
       <c r="F46" s="16"/>
       <c r="G46" s="18"/>
-      <c r="I46" s="53">
+      <c r="I46" s="54">
         <v>117.0</v>
       </c>
-      <c r="J46" s="54"/>
+      <c r="J46" s="55"/>
       <c r="L46" s="18"/>
       <c r="M46" s="16"/>
       <c r="N46" s="18"/>
@@ -3936,19 +3943,19 @@
     </row>
     <row r="47">
       <c r="A47" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B47" s="52" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="55" t="s">
+      <c r="B47" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="46" t="b">
+      <c r="C47" s="56" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="47" t="b">
         <v>1</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G47" s="18"/>
       <c r="I47" s="20"/>
@@ -3967,11 +3974,11 @@
       <c r="A48" s="15">
         <v>235.0</v>
       </c>
-      <c r="B48" s="52" t="s">
-        <v>146</v>
-      </c>
-      <c r="C48" s="45" t="s">
+      <c r="B48" s="53" t="s">
         <v>147</v>
+      </c>
+      <c r="C48" s="46" t="s">
+        <v>148</v>
       </c>
       <c r="D48" s="18"/>
       <c r="E48" s="19"/>
@@ -3995,11 +4002,11 @@
       <c r="A49" s="15">
         <v>236.0</v>
       </c>
-      <c r="B49" s="52" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="45" t="s">
+      <c r="B49" s="53" t="s">
         <v>149</v>
+      </c>
+      <c r="C49" s="46" t="s">
+        <v>150</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="19"/>
@@ -4023,11 +4030,11 @@
       <c r="A50" s="15">
         <v>237.0</v>
       </c>
-      <c r="B50" s="52" t="s">
-        <v>150</v>
+      <c r="B50" s="53" t="s">
+        <v>151</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D50" s="18"/>
       <c r="E50" s="19"/>
@@ -4051,11 +4058,11 @@
       <c r="A51" s="15">
         <v>238.0</v>
       </c>
-      <c r="B51" s="52" t="s">
-        <v>152</v>
+      <c r="B51" s="53" t="s">
+        <v>153</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D51" s="18"/>
       <c r="E51" s="19"/>
@@ -4079,11 +4086,11 @@
       <c r="A52" s="15">
         <v>239.0</v>
       </c>
-      <c r="B52" s="52" t="s">
-        <v>154</v>
+      <c r="B52" s="53" t="s">
+        <v>155</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D52" s="18"/>
       <c r="E52" s="19"/>
@@ -4093,7 +4100,7 @@
         <v>117.0</v>
       </c>
       <c r="J52" s="18"/>
-      <c r="M52" s="40">
+      <c r="M52" s="41">
         <v>249.0</v>
       </c>
       <c r="N52" s="26">
@@ -4111,10 +4118,10 @@
         <v>240.0</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="19"/>
@@ -4124,7 +4131,7 @@
         <v>117.0</v>
       </c>
       <c r="J53" s="18"/>
-      <c r="M53" s="40">
+      <c r="M53" s="41">
         <v>248.0</v>
       </c>
       <c r="N53" s="26">
@@ -4142,10 +4149,10 @@
         <v>241.0</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D54" s="18"/>
       <c r="E54" s="19"/>
@@ -4165,21 +4172,21 @@
       <c r="U54" s="18"/>
     </row>
     <row r="55">
-      <c r="A55" s="56" t="s">
-        <v>160</v>
+      <c r="A55" s="57" t="s">
+        <v>161</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="19"/>
       <c r="F55" s="16"/>
       <c r="G55" s="18"/>
       <c r="I55" s="20"/>
-      <c r="J55" s="40">
+      <c r="J55" s="41">
         <v>114.0</v>
       </c>
       <c r="M55" s="15">
@@ -4196,25 +4203,25 @@
       <c r="U55" s="18"/>
     </row>
     <row r="56">
-      <c r="A56" s="56" t="s">
-        <v>163</v>
+      <c r="A56" s="57" t="s">
+        <v>164</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D56" s="18"/>
       <c r="E56" s="19"/>
       <c r="F56" s="16"/>
       <c r="G56" s="18"/>
       <c r="I56" s="20"/>
-      <c r="J56" s="40">
+      <c r="J56" s="41">
         <v>112.0</v>
       </c>
       <c r="L56" s="16"/>
-      <c r="M56" s="57"/>
+      <c r="M56" s="58"/>
       <c r="N56" s="16"/>
       <c r="O56" s="18"/>
       <c r="P56" s="18"/>
@@ -4224,14 +4231,14 @@
       <c r="U56" s="18"/>
     </row>
     <row r="57">
-      <c r="A57" s="58">
+      <c r="A57" s="59">
         <v>242.0</v>
       </c>
-      <c r="B57" s="52" t="s">
-        <v>166</v>
+      <c r="B57" s="53" t="s">
+        <v>167</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D57" s="18"/>
       <c r="E57" s="19"/>
@@ -4252,14 +4259,14 @@
       <c r="U57" s="18"/>
     </row>
     <row r="58">
-      <c r="A58" s="58">
+      <c r="A58" s="59">
         <v>243.0</v>
       </c>
-      <c r="B58" s="52" t="s">
-        <v>168</v>
+      <c r="B58" s="53" t="s">
+        <v>169</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D58" s="18"/>
       <c r="E58" s="19"/>
@@ -4280,14 +4287,14 @@
       <c r="U58" s="22"/>
     </row>
     <row r="59">
-      <c r="A59" s="58">
+      <c r="A59" s="59">
         <v>244.0</v>
       </c>
-      <c r="B59" s="52" t="s">
-        <v>170</v>
+      <c r="B59" s="53" t="s">
+        <v>171</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D59" s="18"/>
       <c r="E59" s="19"/>
@@ -4306,14 +4313,14 @@
       <c r="U59" s="22"/>
     </row>
     <row r="60">
-      <c r="A60" s="59">
+      <c r="A60" s="60">
         <v>245.0</v>
       </c>
-      <c r="B60" s="52" t="s">
-        <v>172</v>
+      <c r="B60" s="53" t="s">
+        <v>173</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D60" s="18"/>
       <c r="E60" s="19"/>
@@ -4332,14 +4339,14 @@
       <c r="U60" s="22"/>
     </row>
     <row r="61">
-      <c r="A61" s="59">
+      <c r="A61" s="60">
         <v>246.0</v>
       </c>
-      <c r="B61" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="C61" s="60" t="s">
+      <c r="B61" s="53" t="s">
         <v>175</v>
+      </c>
+      <c r="C61" s="61" t="s">
+        <v>176</v>
       </c>
       <c r="D61" s="18"/>
       <c r="E61" s="19"/>
@@ -4358,14 +4365,14 @@
       <c r="U61" s="22"/>
     </row>
     <row r="62">
-      <c r="A62" s="59">
+      <c r="A62" s="60">
         <v>247.0</v>
       </c>
-      <c r="B62" s="52" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" s="60" t="s">
+      <c r="B62" s="53" t="s">
         <v>177</v>
+      </c>
+      <c r="C62" s="61" t="s">
+        <v>178</v>
       </c>
       <c r="D62" s="18"/>
       <c r="E62" s="19"/>
@@ -4384,14 +4391,14 @@
       <c r="U62" s="22"/>
     </row>
     <row r="63">
-      <c r="A63" s="59">
+      <c r="A63" s="60">
         <v>248.0</v>
       </c>
-      <c r="B63" s="52" t="s">
-        <v>178</v>
-      </c>
-      <c r="C63" s="60" t="s">
+      <c r="B63" s="53" t="s">
         <v>179</v>
+      </c>
+      <c r="C63" s="61" t="s">
+        <v>180</v>
       </c>
       <c r="D63" s="18"/>
       <c r="E63" s="19"/>
@@ -4399,7 +4406,7 @@
       <c r="G63" s="18"/>
       <c r="I63" s="20"/>
       <c r="J63" s="16"/>
-      <c r="L63" s="61"/>
+      <c r="L63" s="62"/>
       <c r="M63" s="18"/>
       <c r="N63" s="18"/>
       <c r="O63" s="18"/>
@@ -4410,23 +4417,23 @@
       <c r="U63" s="22"/>
     </row>
     <row r="64">
-      <c r="A64" s="59">
+      <c r="A64" s="60">
         <v>249.0</v>
       </c>
-      <c r="B64" s="52" t="s">
-        <v>180</v>
-      </c>
-      <c r="C64" s="60" t="s">
+      <c r="B64" s="53" t="s">
         <v>181</v>
+      </c>
+      <c r="C64" s="61" t="s">
+        <v>182</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="19"/>
       <c r="F64" s="16"/>
       <c r="G64" s="18"/>
       <c r="I64" s="20"/>
-      <c r="J64" s="62"/>
-      <c r="M64" s="63" t="s">
-        <v>182</v>
+      <c r="J64" s="63"/>
+      <c r="M64" s="64" t="s">
+        <v>183</v>
       </c>
       <c r="N64" s="26">
         <v>0.0</v>
@@ -4439,14 +4446,14 @@
       <c r="U64" s="22"/>
     </row>
     <row r="65">
-      <c r="A65" s="59">
+      <c r="A65" s="60">
         <v>250.0</v>
       </c>
-      <c r="B65" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="C65" s="60" t="s">
+      <c r="B65" s="53" t="s">
         <v>184</v>
+      </c>
+      <c r="C65" s="61" t="s">
+        <v>185</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="19"/>
@@ -4465,14 +4472,14 @@
       <c r="U65" s="22"/>
     </row>
     <row r="66">
-      <c r="A66" s="59">
+      <c r="A66" s="60">
         <v>251.0</v>
       </c>
-      <c r="B66" s="52" t="s">
-        <v>185</v>
-      </c>
-      <c r="C66" s="60" t="s">
+      <c r="B66" s="53" t="s">
         <v>186</v>
+      </c>
+      <c r="C66" s="61" t="s">
+        <v>187</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="19"/>
@@ -4491,14 +4498,14 @@
       <c r="U66" s="22"/>
     </row>
     <row r="67">
-      <c r="A67" s="59">
+      <c r="A67" s="60">
         <v>252.0</v>
       </c>
-      <c r="B67" s="52" t="s">
-        <v>187</v>
-      </c>
-      <c r="C67" s="60" t="s">
+      <c r="B67" s="53" t="s">
         <v>188</v>
+      </c>
+      <c r="C67" s="61" t="s">
+        <v>189</v>
       </c>
       <c r="D67" s="18"/>
       <c r="E67" s="19"/>
@@ -4517,14 +4524,14 @@
       <c r="U67" s="22"/>
     </row>
     <row r="68">
-      <c r="A68" s="59">
+      <c r="A68" s="60">
         <v>253.0</v>
       </c>
-      <c r="B68" s="52" t="s">
-        <v>189</v>
-      </c>
-      <c r="C68" s="60" t="s">
+      <c r="B68" s="53" t="s">
         <v>190</v>
+      </c>
+      <c r="C68" s="61" t="s">
+        <v>191</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="19"/>
@@ -4543,14 +4550,14 @@
       <c r="U68" s="22"/>
     </row>
     <row r="69">
-      <c r="A69" s="59">
+      <c r="A69" s="60">
         <v>254.0</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="C69" s="60" t="s">
         <v>192</v>
+      </c>
+      <c r="C69" s="61" t="s">
+        <v>193</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="19"/>
@@ -4569,14 +4576,14 @@
       <c r="U69" s="22"/>
     </row>
     <row r="70">
-      <c r="A70" s="59">
+      <c r="A70" s="60">
         <v>255.0</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" s="64" t="s">
         <v>194</v>
+      </c>
+      <c r="C70" s="65" t="s">
+        <v>195</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="19"/>
@@ -4595,14 +4602,14 @@
       <c r="U70" s="22"/>
     </row>
     <row r="71">
-      <c r="A71" s="59">
+      <c r="A71" s="60">
         <v>256.0</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D71" s="18"/>
       <c r="E71" s="19"/>
@@ -4621,14 +4628,14 @@
       <c r="U71" s="22"/>
     </row>
     <row r="72">
-      <c r="A72" s="59">
+      <c r="A72" s="60">
         <v>257.0</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="C72" s="60" t="s">
         <v>198</v>
+      </c>
+      <c r="C72" s="61" t="s">
+        <v>199</v>
       </c>
       <c r="D72" s="18"/>
       <c r="E72" s="19"/>
@@ -4647,14 +4654,14 @@
       <c r="U72" s="22"/>
     </row>
     <row r="73">
-      <c r="A73" s="59">
+      <c r="A73" s="60">
         <v>258.0</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="C73" s="60" t="s">
         <v>200</v>
+      </c>
+      <c r="C73" s="61" t="s">
+        <v>201</v>
       </c>
       <c r="D73" s="18"/>
       <c r="E73" s="19"/>
@@ -4673,14 +4680,14 @@
       <c r="U73" s="22"/>
     </row>
     <row r="74">
-      <c r="A74" s="59">
+      <c r="A74" s="60">
         <v>259.0</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="C74" s="65" t="s">
         <v>202</v>
+      </c>
+      <c r="C74" s="66" t="s">
+        <v>203</v>
       </c>
       <c r="D74" s="18"/>
       <c r="E74" s="19"/>
@@ -4699,14 +4706,14 @@
       <c r="U74" s="22"/>
     </row>
     <row r="75">
-      <c r="A75" s="59">
+      <c r="A75" s="60">
         <v>260.0</v>
       </c>
-      <c r="B75" s="66" t="s">
-        <v>203</v>
+      <c r="B75" s="67" t="s">
+        <v>204</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D75" s="18"/>
       <c r="E75" s="19"/>
@@ -4721,21 +4728,21 @@
       <c r="P75" s="21"/>
       <c r="Q75" s="18"/>
       <c r="R75" s="22"/>
-      <c r="S75" s="67" t="s">
-        <v>205</v>
+      <c r="S75" s="68" t="s">
+        <v>206</v>
       </c>
       <c r="T75" s="22"/>
       <c r="U75" s="22"/>
     </row>
     <row r="76">
-      <c r="A76" s="59">
+      <c r="A76" s="60">
         <v>261.0</v>
       </c>
-      <c r="B76" s="66" t="s">
-        <v>206</v>
+      <c r="B76" s="67" t="s">
+        <v>207</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="19"/>
@@ -4750,21 +4757,21 @@
       <c r="P76" s="21"/>
       <c r="Q76" s="18"/>
       <c r="R76" s="22"/>
-      <c r="S76" s="67" t="s">
-        <v>205</v>
+      <c r="S76" s="68" t="s">
+        <v>206</v>
       </c>
       <c r="T76" s="22"/>
       <c r="U76" s="22"/>
     </row>
     <row r="77">
-      <c r="A77" s="68" t="s">
-        <v>208</v>
+      <c r="A77" s="69" t="s">
+        <v>209</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="C77" s="60" t="s">
         <v>210</v>
+      </c>
+      <c r="C77" s="61" t="s">
+        <v>211</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="19"/>
@@ -4775,10 +4782,10 @@
         <v>107.0</v>
       </c>
       <c r="M77" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="N77" s="26" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="O77" s="18"/>
       <c r="P77" s="21"/>
@@ -4788,14 +4795,14 @@
       <c r="U77" s="22"/>
     </row>
     <row r="78">
-      <c r="A78" s="68" t="s">
-        <v>213</v>
+      <c r="A78" s="69" t="s">
+        <v>214</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="C78" s="60" t="s">
         <v>215</v>
+      </c>
+      <c r="C78" s="61" t="s">
+        <v>216</v>
       </c>
       <c r="D78" s="18"/>
       <c r="E78" s="19"/>
@@ -4819,14 +4826,14 @@
       <c r="U78" s="22"/>
     </row>
     <row r="79">
-      <c r="A79" s="68" t="s">
-        <v>216</v>
+      <c r="A79" s="69" t="s">
+        <v>217</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C79" s="60" t="s">
         <v>218</v>
+      </c>
+      <c r="C79" s="61" t="s">
+        <v>219</v>
       </c>
       <c r="D79" s="18"/>
       <c r="E79" s="19"/>
@@ -4850,14 +4857,14 @@
       <c r="U79" s="22"/>
     </row>
     <row r="80">
-      <c r="A80" s="59">
+      <c r="A80" s="60">
         <v>262.0</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>219</v>
-      </c>
-      <c r="C80" s="60" t="s">
         <v>220</v>
+      </c>
+      <c r="C80" s="61" t="s">
+        <v>221</v>
       </c>
       <c r="D80" s="18"/>
       <c r="E80" s="19"/>
@@ -4877,14 +4884,14 @@
       <c r="U80" s="22"/>
     </row>
     <row r="81">
-      <c r="A81" s="59">
+      <c r="A81" s="60">
         <v>263.0</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="C81" s="60" t="s">
         <v>222</v>
+      </c>
+      <c r="C81" s="61" t="s">
+        <v>223</v>
       </c>
       <c r="D81" s="18"/>
       <c r="E81" s="19"/>
@@ -4904,14 +4911,14 @@
       <c r="U81" s="22"/>
     </row>
     <row r="82">
-      <c r="A82" s="59">
+      <c r="A82" s="60">
         <v>264.0</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C82" s="60" t="s">
         <v>224</v>
+      </c>
+      <c r="C82" s="61" t="s">
+        <v>225</v>
       </c>
       <c r="D82" s="18"/>
       <c r="E82" s="19"/>
@@ -4931,14 +4938,14 @@
       <c r="U82" s="22"/>
     </row>
     <row r="83">
-      <c r="A83" s="59">
+      <c r="A83" s="60">
         <v>265.0</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>225</v>
-      </c>
-      <c r="C83" s="60" t="s">
         <v>226</v>
+      </c>
+      <c r="C83" s="61" t="s">
+        <v>227</v>
       </c>
       <c r="D83" s="18"/>
       <c r="E83" s="19"/>
@@ -4946,9 +4953,9 @@
       <c r="G83" s="18"/>
       <c r="I83" s="20"/>
       <c r="J83" s="16"/>
-      <c r="K83" s="69"/>
+      <c r="K83" s="70"/>
       <c r="M83" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N83" s="26">
         <v>0.0</v>
@@ -4961,14 +4968,14 @@
       <c r="U83" s="22"/>
     </row>
     <row r="84">
-      <c r="A84" s="59">
+      <c r="A84" s="60">
         <v>266.0</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>228</v>
-      </c>
-      <c r="C84" s="60" t="s">
         <v>229</v>
+      </c>
+      <c r="C84" s="61" t="s">
+        <v>230</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="19"/>
@@ -4976,9 +4983,9 @@
       <c r="G84" s="18"/>
       <c r="I84" s="20"/>
       <c r="J84" s="16"/>
-      <c r="K84" s="69"/>
+      <c r="K84" s="70"/>
       <c r="M84" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N84" s="26">
         <v>0.0</v>
@@ -4991,14 +4998,14 @@
       <c r="U84" s="22"/>
     </row>
     <row r="85">
-      <c r="A85" s="68" t="s">
-        <v>231</v>
+      <c r="A85" s="69" t="s">
+        <v>232</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>232</v>
-      </c>
-      <c r="C85" s="60" t="s">
         <v>233</v>
+      </c>
+      <c r="C85" s="61" t="s">
+        <v>234</v>
       </c>
       <c r="D85" s="18"/>
       <c r="E85" s="19"/>
@@ -5008,7 +5015,7 @@
       <c r="J85" s="15">
         <v>108.0</v>
       </c>
-      <c r="K85" s="69"/>
+      <c r="K85" s="70"/>
       <c r="M85" s="15">
         <v>257.0</v>
       </c>
@@ -5023,14 +5030,14 @@
       <c r="U85" s="22"/>
     </row>
     <row r="86">
-      <c r="A86" s="68" t="s">
-        <v>234</v>
+      <c r="A86" s="69" t="s">
+        <v>235</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>235</v>
-      </c>
-      <c r="C86" s="60" t="s">
         <v>236</v>
+      </c>
+      <c r="C86" s="61" t="s">
+        <v>237</v>
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="19"/>
@@ -5040,7 +5047,7 @@
       <c r="J86" s="15">
         <v>109.0</v>
       </c>
-      <c r="K86" s="69"/>
+      <c r="K86" s="70"/>
       <c r="L86" s="16"/>
       <c r="M86" s="16"/>
       <c r="N86" s="18"/>
@@ -5056,10 +5063,10 @@
         <v>57</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>237</v>
-      </c>
-      <c r="C87" s="70" t="s">
         <v>238</v>
+      </c>
+      <c r="C87" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D87" s="18"/>
       <c r="E87" s="19"/>
@@ -5069,7 +5076,7 @@
       <c r="J87" s="15">
         <v>229.0</v>
       </c>
-      <c r="K87" s="69"/>
+      <c r="K87" s="70"/>
       <c r="L87" s="16"/>
       <c r="M87" s="16"/>
       <c r="N87" s="18"/>
@@ -5077,20 +5084,20 @@
       <c r="P87" s="18"/>
       <c r="Q87" s="21"/>
       <c r="R87" s="18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="T87" s="22"/>
       <c r="U87" s="22"/>
     </row>
     <row r="88">
       <c r="A88" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="C88" s="70" t="s">
-        <v>238</v>
+        <v>241</v>
+      </c>
+      <c r="C88" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D88" s="18"/>
       <c r="E88" s="19"/>
@@ -5100,7 +5107,7 @@
       <c r="J88" s="15">
         <v>229.0</v>
       </c>
-      <c r="K88" s="69"/>
+      <c r="K88" s="70"/>
       <c r="L88" s="16"/>
       <c r="M88" s="16"/>
       <c r="N88" s="18"/>
@@ -5108,20 +5115,20 @@
       <c r="P88" s="18"/>
       <c r="Q88" s="21"/>
       <c r="R88" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="T88" s="22"/>
       <c r="U88" s="22"/>
     </row>
     <row r="89">
       <c r="A89" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="C89" s="70" t="s">
-        <v>238</v>
+        <v>243</v>
+      </c>
+      <c r="C89" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D89" s="18"/>
       <c r="E89" s="19"/>
@@ -5131,7 +5138,7 @@
       <c r="J89" s="15">
         <v>229.0</v>
       </c>
-      <c r="K89" s="69"/>
+      <c r="K89" s="70"/>
       <c r="L89" s="16"/>
       <c r="M89" s="16"/>
       <c r="N89" s="18"/>
@@ -5139,20 +5146,20 @@
       <c r="P89" s="18"/>
       <c r="Q89" s="21"/>
       <c r="R89" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="T89" s="22"/>
       <c r="U89" s="22"/>
     </row>
     <row r="90">
       <c r="A90" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="C90" s="70" t="s">
-        <v>238</v>
+        <v>245</v>
+      </c>
+      <c r="C90" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D90" s="18"/>
       <c r="E90" s="19"/>
@@ -5160,7 +5167,7 @@
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
       <c r="I90" s="20"/>
-      <c r="J90" s="40">
+      <c r="J90" s="41">
         <v>229.0</v>
       </c>
       <c r="K90" s="38"/>
@@ -5176,13 +5183,13 @@
     </row>
     <row r="91">
       <c r="A91" s="27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="C91" s="70" t="s">
-        <v>238</v>
+        <v>246</v>
+      </c>
+      <c r="C91" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D91" s="18"/>
       <c r="E91" s="19"/>
@@ -5192,7 +5199,7 @@
       <c r="J91" s="15">
         <v>229.0</v>
       </c>
-      <c r="K91" s="69"/>
+      <c r="K91" s="70"/>
       <c r="L91" s="16"/>
       <c r="M91" s="16"/>
       <c r="N91" s="18"/>
@@ -5200,21 +5207,21 @@
       <c r="P91" s="18"/>
       <c r="Q91" s="21"/>
       <c r="R91" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="T91" s="22"/>
       <c r="U91" s="22"/>
     </row>
     <row r="92">
       <c r="A92" s="27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B92" s="13" t="str">
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A92,1),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (4) (bolew)</v>
       </c>
-      <c r="C92" s="70" t="s">
-        <v>238</v>
+      <c r="C92" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D92" s="18"/>
       <c r="E92" s="19"/>
@@ -5224,7 +5231,7 @@
       <c r="J92" s="15">
         <v>229.0</v>
       </c>
-      <c r="K92" s="69"/>
+      <c r="K92" s="70"/>
       <c r="L92" s="16"/>
       <c r="M92" s="16"/>
       <c r="N92" s="18"/>
@@ -5232,21 +5239,21 @@
       <c r="P92" s="18"/>
       <c r="Q92" s="21"/>
       <c r="R92" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="T92" s="22"/>
       <c r="U92" s="22"/>
     </row>
     <row r="93">
       <c r="A93" s="27" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B93" s="13" t="str">
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A93,2),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (10) (bolew)</v>
       </c>
-      <c r="C93" s="70" t="s">
-        <v>238</v>
+      <c r="C93" s="71" t="s">
+        <v>239</v>
       </c>
       <c r="D93" s="18"/>
       <c r="E93" s="19"/>
@@ -5256,7 +5263,7 @@
       <c r="J93" s="15">
         <v>229.0</v>
       </c>
-      <c r="K93" s="69"/>
+      <c r="K93" s="70"/>
       <c r="L93" s="16"/>
       <c r="M93" s="16"/>
       <c r="N93" s="18"/>
@@ -5264,31 +5271,31 @@
       <c r="P93" s="18"/>
       <c r="Q93" s="21"/>
       <c r="R93" s="18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="T93" s="22"/>
       <c r="U93" s="22"/>
     </row>
     <row r="94">
-      <c r="A94" s="71" t="s">
-        <v>251</v>
+      <c r="A94" s="72" t="s">
+        <v>252</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="C94" s="70"/>
+        <v>253</v>
+      </c>
+      <c r="C94" s="71"/>
       <c r="D94" s="18"/>
       <c r="E94" s="19"/>
       <c r="F94" s="16"/>
       <c r="G94" s="18"/>
       <c r="I94" s="20"/>
       <c r="J94" s="15"/>
-      <c r="K94" s="69"/>
+      <c r="K94" s="70"/>
       <c r="M94" s="26" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="N94" s="26" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O94" s="18"/>
       <c r="P94" s="18"/>
@@ -5319,16 +5326,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="73" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5337,49 +5344,49 @@
         <v>104.0</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="C2" s="74" t="s">
         <v>256</v>
       </c>
-      <c r="D2" s="75"/>
+      <c r="C2" s="75" t="s">
+        <v>257</v>
+      </c>
+      <c r="D2" s="76"/>
     </row>
     <row r="3">
       <c r="A3" s="15">
         <v>105.0</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>258</v>
-      </c>
-      <c r="D3" s="75"/>
+        <v>259</v>
+      </c>
+      <c r="D3" s="76"/>
     </row>
     <row r="4">
       <c r="A4" s="15">
         <v>107.0</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="D4" s="40"/>
+        <v>261</v>
+      </c>
+      <c r="D4" s="41"/>
     </row>
     <row r="5">
       <c r="A5" s="15">
         <v>53.0</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="D5" s="76" t="s">
         <v>263</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="6">
@@ -5387,10 +5394,10 @@
         <v>48.0</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D6" s="18"/>
     </row>
@@ -5399,10 +5406,10 @@
         <v>49.0</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>266</v>
-      </c>
-      <c r="C7" s="77" t="s">
         <v>267</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>268</v>
       </c>
       <c r="D7" s="18"/>
     </row>
@@ -5411,10 +5418,10 @@
         <v>50.0</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>268</v>
-      </c>
-      <c r="C8" s="77" t="s">
         <v>269</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>270</v>
       </c>
       <c r="D8" s="18"/>
     </row>
@@ -5423,10 +5430,10 @@
         <v>51.0</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="C9" s="77" t="s">
         <v>271</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>272</v>
       </c>
       <c r="D9" s="18"/>
     </row>
@@ -5435,10 +5442,10 @@
         <v>52.0</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D10" s="18"/>
     </row>
@@ -5447,10 +5454,10 @@
         <v>83.0</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D11" s="18"/>
     </row>
@@ -5459,10 +5466,10 @@
         <v>84.0</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D12" s="18"/>
     </row>
@@ -5471,12 +5478,12 @@
         <v>54.0</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="D13" s="40">
+        <v>280</v>
+      </c>
+      <c r="D13" s="41">
         <v>53.0</v>
       </c>
     </row>
@@ -5485,10 +5492,10 @@
         <v>55.0</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D14" s="18"/>
     </row>
@@ -5497,12 +5504,12 @@
         <v>56.0</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>283</v>
-      </c>
-      <c r="D15" s="40">
+        <v>284</v>
+      </c>
+      <c r="D15" s="41">
         <v>55.0</v>
       </c>
     </row>
@@ -5511,10 +5518,10 @@
         <v>85.0</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D16" s="18"/>
     </row>
@@ -5523,10 +5530,10 @@
         <v>2.0</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>286</v>
-      </c>
-      <c r="C17" s="78" t="s">
         <v>287</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>288</v>
       </c>
       <c r="D17" s="18"/>
     </row>
@@ -5535,10 +5542,10 @@
         <v>42.0</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>288</v>
-      </c>
-      <c r="C18" s="45" t="s">
         <v>289</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>290</v>
       </c>
       <c r="D18" s="18"/>
     </row>
@@ -5547,12 +5554,12 @@
         <v>41.0</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>290</v>
-      </c>
-      <c r="C19" s="45" t="s">
         <v>291</v>
       </c>
-      <c r="D19" s="40">
+      <c r="C19" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="D19" s="41">
         <v>53.0</v>
       </c>
     </row>
@@ -5561,24 +5568,24 @@
         <v>100.0</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>292</v>
-      </c>
-      <c r="C20" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="C20" s="49" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" s="41"/>
     </row>
     <row r="21">
       <c r="A21" s="15">
         <v>101.0</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>295</v>
-      </c>
-      <c r="D21" s="40">
+        <v>296</v>
+      </c>
+      <c r="D21" s="41">
         <v>100.0</v>
       </c>
     </row>
@@ -5587,12 +5594,12 @@
         <v>102.0</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>296</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>262</v>
-      </c>
-      <c r="D22" s="40">
+        <v>297</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>263</v>
+      </c>
+      <c r="D22" s="41">
         <v>100.0</v>
       </c>
     </row>
@@ -5601,12 +5608,12 @@
         <v>103.0</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>298</v>
-      </c>
-      <c r="D23" s="40">
+        <v>299</v>
+      </c>
+      <c r="D23" s="41">
         <v>101.0</v>
       </c>
     </row>
@@ -5615,12 +5622,12 @@
         <v>106.0</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="D24" s="40">
+        <v>301</v>
+      </c>
+      <c r="D24" s="41">
         <v>111.0</v>
       </c>
     </row>
@@ -5629,12 +5636,12 @@
         <v>108.0</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="D25" s="40">
+        <v>302</v>
+      </c>
+      <c r="D25" s="41">
         <v>111.0</v>
       </c>
     </row>
@@ -5643,12 +5650,12 @@
         <v>109.0</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="D26" s="40">
+        <v>304</v>
+      </c>
+      <c r="D26" s="41">
         <v>111.0</v>
       </c>
     </row>
@@ -5657,12 +5664,12 @@
         <v>110.0</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>305</v>
-      </c>
-      <c r="D27" s="40">
+        <v>306</v>
+      </c>
+      <c r="D27" s="41">
         <v>111.0</v>
       </c>
     </row>
@@ -5671,10 +5678,10 @@
         <v>111.0</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D28" s="18"/>
     </row>
@@ -5683,10 +5690,10 @@
         <v>112.0</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D29" s="18"/>
     </row>
@@ -5695,10 +5702,10 @@
         <v>113.0</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D30" s="18"/>
     </row>
@@ -5707,10 +5714,10 @@
         <v>114.0</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D31" s="18"/>
     </row>
@@ -5719,10 +5726,10 @@
         <v>115.0</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D32" s="18"/>
     </row>
@@ -5731,12 +5738,12 @@
         <v>116.0</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>315</v>
-      </c>
-      <c r="D33" s="40">
+        <v>316</v>
+      </c>
+      <c r="D33" s="41">
         <v>53.0</v>
       </c>
     </row>
@@ -5745,12 +5752,12 @@
         <v>117.0</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>317</v>
-      </c>
-      <c r="D34" s="40">
+        <v>318</v>
+      </c>
+      <c r="D34" s="41">
         <v>116.0</v>
       </c>
     </row>
@@ -5778,38 +5785,38 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
-        <v>318</v>
-      </c>
-      <c r="D1" s="79" t="s">
+      <c r="C1" s="80" t="s">
         <v>319</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="D1" s="80" t="s">
         <v>320</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="E1" s="80" t="s">
+        <v>321</v>
+      </c>
+      <c r="F1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="79" t="s">
-        <v>321</v>
+      <c r="G1" s="80" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="21" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>57</v>
@@ -5818,97 +5825,97 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B3" s="16"/>
       <c r="C3" s="21" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="G3" s="22"/>
     </row>
     <row r="4">
       <c r="A4" s="27" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B4" s="16"/>
       <c r="C4" s="27" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G4" s="22"/>
     </row>
     <row r="5">
-      <c r="A5" s="71" t="s">
-        <v>331</v>
+      <c r="A5" s="72" t="s">
+        <v>332</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="27" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G5" s="22"/>
     </row>
     <row r="6">
       <c r="A6" s="27" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="27" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="G6" s="22"/>
     </row>
     <row r="7">
       <c r="A7" s="27" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="27" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G7" s="22"/>
     </row>
     <row r="8">
       <c r="A8" s="27" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="27" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G8" s="22"/>
     </row>
@@ -5950,72 +5957,72 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="79" t="s">
-        <v>343</v>
-      </c>
-      <c r="E1" s="79" t="s">
+      <c r="D1" s="80" t="s">
         <v>344</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="E1" s="80" t="s">
         <v>345</v>
       </c>
-      <c r="G1" s="79" t="s">
+      <c r="F1" s="81" t="s">
         <v>346</v>
       </c>
-      <c r="H1" s="79" t="s">
+      <c r="G1" s="80" t="s">
+        <v>347</v>
+      </c>
+      <c r="H1" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="79" t="s">
-        <v>347</v>
-      </c>
-      <c r="J1" s="81" t="s">
+      <c r="I1" s="80" t="s">
         <v>348</v>
       </c>
-      <c r="K1" s="79" t="s">
+      <c r="J1" s="82" t="s">
         <v>349</v>
       </c>
-      <c r="L1" s="82" t="s">
+      <c r="K1" s="80" t="s">
         <v>350</v>
       </c>
-      <c r="M1" s="83" t="s">
-        <v>321</v>
-      </c>
-      <c r="N1" s="83" t="s">
+      <c r="L1" s="83" t="s">
+        <v>351</v>
+      </c>
+      <c r="M1" s="84" t="s">
+        <v>322</v>
+      </c>
+      <c r="N1" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="83" t="s">
+      <c r="O1" s="84" t="s">
         <v>23</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
-      <c r="D2" s="71" t="s">
-        <v>353</v>
+      <c r="D2" s="72" t="s">
+        <v>354</v>
       </c>
       <c r="E2" s="22"/>
-      <c r="F2" s="84" t="s">
-        <v>354</v>
+      <c r="F2" s="85" t="s">
+        <v>355</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>355</v>
-      </c>
-      <c r="H2" s="85"/>
+        <v>356</v>
+      </c>
+      <c r="H2" s="86"/>
       <c r="I2" s="22"/>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
@@ -6023,7 +6030,7 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
       <c r="O2" s="14" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="P2" s="14" t="b">
         <v>1</v>
@@ -6031,20 +6038,20 @@
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B3" s="14"/>
       <c r="D3" s="30" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="E3" s="22"/>
-      <c r="F3" s="84" t="s">
-        <v>359</v>
+      <c r="F3" s="85" t="s">
+        <v>360</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>360</v>
-      </c>
-      <c r="H3" s="85"/>
+        <v>361</v>
+      </c>
+      <c r="H3" s="86"/>
       <c r="I3" s="22"/>
       <c r="J3" s="22"/>
       <c r="K3" s="22"/>
@@ -6052,7 +6059,7 @@
       <c r="M3" s="22"/>
       <c r="N3" s="22"/>
       <c r="O3" s="14" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="P3" s="14" t="b">
         <v>1</v>
@@ -6060,51 +6067,47 @@
     </row>
     <row r="4">
       <c r="A4" s="26" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B4" s="16"/>
-      <c r="D4" s="86" t="s">
-        <v>363</v>
-      </c>
-      <c r="E4" s="47"/>
-      <c r="F4" s="87" t="s">
+      <c r="D4" s="87" t="s">
         <v>364</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="E4" s="48"/>
+      <c r="F4" s="88" t="s">
         <v>365</v>
       </c>
+      <c r="G4" s="88" t="s">
+        <v>366</v>
+      </c>
       <c r="H4" s="16"/>
-      <c r="I4" s="47"/>
+      <c r="I4" s="48"/>
       <c r="J4" s="16"/>
       <c r="K4" s="30"/>
       <c r="L4" s="18"/>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
-      <c r="O4" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="P4" s="14" t="b">
-        <v>1</v>
-      </c>
+      <c r="O4" s="39"/>
+      <c r="P4" s="39"/>
     </row>
     <row r="5">
       <c r="A5" s="26" t="s">
         <v>367</v>
       </c>
       <c r="B5" s="16"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="89" t="s">
+      <c r="C5" s="89"/>
+      <c r="D5" s="90" t="s">
         <v>368</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="87" t="s">
+      <c r="E5" s="48"/>
+      <c r="F5" s="88" t="s">
         <v>369</v>
       </c>
-      <c r="G5" s="87" t="s">
+      <c r="G5" s="88" t="s">
         <v>370</v>
       </c>
       <c r="H5" s="16"/>
-      <c r="I5" s="47"/>
+      <c r="I5" s="48"/>
       <c r="J5" s="16"/>
       <c r="K5" s="30"/>
       <c r="L5" s="18"/>
@@ -6122,19 +6125,19 @@
         <v>372</v>
       </c>
       <c r="B6" s="16"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="90">
+      <c r="C6" s="89"/>
+      <c r="D6" s="91">
         <v>227.0</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="87" t="s">
+      <c r="E6" s="48"/>
+      <c r="F6" s="88" t="s">
         <v>373</v>
       </c>
-      <c r="G6" s="87" t="s">
+      <c r="G6" s="88" t="s">
         <v>374</v>
       </c>
       <c r="H6" s="16"/>
-      <c r="I6" s="47"/>
+      <c r="I6" s="48"/>
       <c r="J6" s="16"/>
       <c r="K6" s="30"/>
       <c r="L6" s="18"/>
@@ -6152,49 +6155,53 @@
         <v>376</v>
       </c>
       <c r="B7" s="16"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="90">
+      <c r="C7" s="89"/>
+      <c r="D7" s="91">
         <v>259.0</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="87" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="88" t="s">
         <v>377</v>
       </c>
-      <c r="G7" s="87" t="s">
+      <c r="G7" s="88" t="s">
         <v>378</v>
       </c>
       <c r="H7" s="16"/>
-      <c r="I7" s="47"/>
+      <c r="I7" s="48"/>
       <c r="J7" s="16"/>
       <c r="K7" s="30"/>
       <c r="L7" s="18"/>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
+      <c r="O7" s="39" t="s">
+        <v>379</v>
+      </c>
+      <c r="P7" s="39" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="16" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>380</v>
-      </c>
-      <c r="C8" s="88" t="s">
         <v>381</v>
       </c>
-      <c r="D8" s="91"/>
-      <c r="E8" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F8" s="92" t="s">
-        <v>326</v>
-      </c>
-      <c r="G8" s="87" t="s">
+      <c r="C8" s="89" t="s">
         <v>382</v>
       </c>
+      <c r="D8" s="92"/>
+      <c r="E8" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="93" t="s">
+        <v>327</v>
+      </c>
+      <c r="G8" s="88" t="s">
+        <v>383</v>
+      </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="47"/>
+      <c r="I8" s="48"/>
       <c r="J8" s="16"/>
       <c r="K8" s="30">
         <v>0.0</v>
@@ -6209,32 +6216,32 @@
     </row>
     <row r="9">
       <c r="A9" s="16" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>384</v>
-      </c>
-      <c r="C9" s="88" t="s">
         <v>385</v>
       </c>
-      <c r="D9" s="91"/>
-      <c r="E9" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="92" t="s">
-        <v>327</v>
-      </c>
-      <c r="G9" s="87" t="s">
+      <c r="C9" s="89" t="s">
         <v>386</v>
       </c>
+      <c r="D9" s="92"/>
+      <c r="E9" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="93" t="s">
+        <v>328</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>387</v>
+      </c>
       <c r="H9" s="16"/>
-      <c r="I9" s="93"/>
+      <c r="I9" s="94"/>
       <c r="J9" s="18"/>
-      <c r="K9" s="94" t="s">
-        <v>387</v>
-      </c>
-      <c r="L9" s="93" t="s">
+      <c r="K9" s="95" t="s">
         <v>388</v>
+      </c>
+      <c r="L9" s="94" t="s">
+        <v>389</v>
       </c>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
@@ -6243,30 +6250,30 @@
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>390</v>
-      </c>
-      <c r="C10" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="D10" s="95"/>
-      <c r="E10" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10" s="95" t="s">
-        <v>329</v>
-      </c>
-      <c r="G10" s="96" t="s">
         <v>391</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>382</v>
+      </c>
+      <c r="D10" s="96"/>
+      <c r="E10" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="96" t="s">
+        <v>330</v>
+      </c>
+      <c r="G10" s="97" t="s">
+        <v>392</v>
       </c>
       <c r="H10" s="16"/>
       <c r="J10" s="18"/>
       <c r="K10" s="14">
         <v>0.0</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="42">
         <v>265.0</v>
       </c>
       <c r="M10" s="22"/>
@@ -6276,31 +6283,31 @@
     </row>
     <row r="11">
       <c r="A11" s="16" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>393</v>
-      </c>
-      <c r="C11" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="D11" s="92"/>
-      <c r="E11" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="F11" s="92" t="s">
-        <v>330</v>
+        <v>394</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="D11" s="93"/>
+      <c r="E11" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F11" s="93" t="s">
+        <v>331</v>
       </c>
       <c r="G11" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H11" s="16"/>
       <c r="J11" s="18"/>
       <c r="K11" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="L11" s="97" t="s">
         <v>396</v>
+      </c>
+      <c r="L11" s="98" t="s">
+        <v>397</v>
       </c>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
@@ -6309,30 +6316,30 @@
     </row>
     <row r="12">
       <c r="A12" s="16" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>398</v>
-      </c>
-      <c r="C12" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="D12" s="95"/>
-      <c r="E12" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="95" t="s">
-        <v>332</v>
-      </c>
-      <c r="G12" s="96" t="s">
         <v>399</v>
+      </c>
+      <c r="C12" s="89" t="s">
+        <v>382</v>
+      </c>
+      <c r="D12" s="96"/>
+      <c r="E12" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="96" t="s">
+        <v>333</v>
+      </c>
+      <c r="G12" s="97" t="s">
+        <v>400</v>
       </c>
       <c r="H12" s="16"/>
       <c r="J12" s="18"/>
       <c r="K12" s="14">
         <v>0.0</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="42">
         <v>266.0</v>
       </c>
       <c r="M12" s="22"/>
@@ -6342,31 +6349,31 @@
     </row>
     <row r="13">
       <c r="A13" s="16" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>401</v>
-      </c>
-      <c r="C13" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="D13" s="92"/>
-      <c r="E13" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="F13" s="92" t="s">
-        <v>333</v>
+        <v>402</v>
+      </c>
+      <c r="C13" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="D13" s="93"/>
+      <c r="E13" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F13" s="93" t="s">
+        <v>334</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H13" s="16"/>
       <c r="J13" s="18"/>
       <c r="K13" s="14" t="s">
-        <v>395</v>
-      </c>
-      <c r="L13" s="97" t="s">
-        <v>402</v>
+        <v>396</v>
+      </c>
+      <c r="L13" s="98" t="s">
+        <v>403</v>
       </c>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
@@ -6375,48 +6382,48 @@
     </row>
     <row r="14">
       <c r="A14" s="26" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>404</v>
-      </c>
-      <c r="C14" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E14" s="47" t="s">
-        <v>116</v>
+        <v>405</v>
+      </c>
+      <c r="C14" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>117</v>
       </c>
       <c r="F14" s="30" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="K14" s="30">
         <v>0.0</v>
       </c>
-      <c r="L14" s="98">
+      <c r="L14" s="99">
         <v>261.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="18" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="C15" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>122</v>
-      </c>
-      <c r="F15" s="99" t="s">
-        <v>323</v>
-      </c>
-      <c r="G15" s="87" t="s">
         <v>408</v>
+      </c>
+      <c r="C15" s="89" t="s">
+        <v>382</v>
+      </c>
+      <c r="E15" s="48" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" s="100" t="s">
+        <v>324</v>
+      </c>
+      <c r="G15" s="88" t="s">
+        <v>409</v>
       </c>
       <c r="H15" s="18"/>
       <c r="J15" s="18"/>
@@ -6429,58 +6436,58 @@
     </row>
     <row r="16">
       <c r="A16" s="18" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="C16" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" s="100" t="s">
-        <v>324</v>
-      </c>
-      <c r="G16" s="101" t="s">
         <v>411</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E16" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="101" t="s">
+        <v>325</v>
+      </c>
+      <c r="G16" s="102" t="s">
+        <v>412</v>
       </c>
       <c r="H16" s="18"/>
       <c r="J16" s="18"/>
       <c r="K16" s="30" t="s">
-        <v>412</v>
-      </c>
-      <c r="L16" s="56" t="s">
         <v>413</v>
+      </c>
+      <c r="L16" s="57" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="16" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>415</v>
-      </c>
-      <c r="C17" s="102" t="s">
-        <v>381</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>122</v>
+        <v>416</v>
+      </c>
+      <c r="C17" s="103" t="s">
+        <v>382</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>123</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G17" s="26" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H17" s="16"/>
       <c r="J17" s="18"/>
       <c r="K17" s="14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
@@ -6489,30 +6496,30 @@
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>419</v>
-      </c>
-      <c r="C18" s="102" t="s">
-        <v>385</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>116</v>
+        <v>420</v>
+      </c>
+      <c r="C18" s="103" t="s">
+        <v>386</v>
+      </c>
+      <c r="E18" s="48" t="s">
+        <v>117</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="G18" s="26" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H18" s="16"/>
       <c r="J18" s="18"/>
       <c r="K18" s="14" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
@@ -6521,22 +6528,22 @@
     </row>
     <row r="19">
       <c r="A19" s="16" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>424</v>
-      </c>
-      <c r="C19" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="E19" s="47" t="s">
-        <v>122</v>
+        <v>425</v>
+      </c>
+      <c r="C19" s="89" t="s">
+        <v>382</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>123</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>341</v>
-      </c>
-      <c r="G19" s="71" t="s">
-        <v>425</v>
+        <v>342</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>426</v>
       </c>
       <c r="H19" s="16"/>
       <c r="J19" s="18"/>
@@ -6553,30 +6560,30 @@
     </row>
     <row r="20">
       <c r="A20" s="16" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>427</v>
-      </c>
-      <c r="C20" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E20" s="47" t="s">
-        <v>116</v>
+        <v>428</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>117</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>342</v>
-      </c>
-      <c r="G20" s="71" t="s">
-        <v>428</v>
+        <v>343</v>
+      </c>
+      <c r="G20" s="72" t="s">
+        <v>429</v>
       </c>
       <c r="H20" s="16"/>
       <c r="J20" s="18"/>
       <c r="K20" s="14" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
@@ -6585,22 +6592,22 @@
     </row>
     <row r="21">
       <c r="A21" s="16" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>432</v>
-      </c>
-      <c r="C21" s="88" t="s">
-        <v>381</v>
-      </c>
-      <c r="E21" s="47" t="s">
-        <v>122</v>
+        <v>433</v>
+      </c>
+      <c r="C21" s="89" t="s">
+        <v>382</v>
+      </c>
+      <c r="E21" s="48" t="s">
+        <v>123</v>
       </c>
       <c r="F21" s="27" t="s">
-        <v>338</v>
-      </c>
-      <c r="G21" s="71" t="s">
-        <v>433</v>
+        <v>339</v>
+      </c>
+      <c r="G21" s="72" t="s">
+        <v>434</v>
       </c>
       <c r="H21" s="16"/>
       <c r="J21" s="18"/>
@@ -6617,30 +6624,30 @@
     </row>
     <row r="22">
       <c r="A22" s="16" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>435</v>
-      </c>
-      <c r="C22" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E22" s="47" t="s">
-        <v>116</v>
+        <v>436</v>
+      </c>
+      <c r="C22" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E22" s="48" t="s">
+        <v>117</v>
       </c>
       <c r="F22" s="27" t="s">
-        <v>339</v>
-      </c>
-      <c r="G22" s="71" t="s">
-        <v>436</v>
+        <v>340</v>
+      </c>
+      <c r="G22" s="72" t="s">
+        <v>437</v>
       </c>
       <c r="H22" s="16"/>
       <c r="J22" s="18"/>
       <c r="K22" s="14" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
@@ -6649,158 +6656,158 @@
     </row>
     <row r="23">
       <c r="A23" s="30" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>440</v>
-      </c>
-      <c r="C23" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E23" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="71" t="s">
-        <v>436</v>
+        <v>441</v>
+      </c>
+      <c r="C23" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="72" t="s">
+        <v>437</v>
       </c>
       <c r="G23" s="30" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="K23" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="L23" s="103">
+      <c r="L23" s="104">
         <v>242243.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="30" t="s">
+        <v>443</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>444</v>
+      </c>
+      <c r="C24" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F24" s="30" t="s">
         <v>442</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>443</v>
-      </c>
-      <c r="C24" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E24" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>441</v>
-      </c>
       <c r="G24" s="30" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="L24" s="103" t="s">
         <v>446</v>
+      </c>
+      <c r="L24" s="104" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="30" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>448</v>
-      </c>
-      <c r="C25" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E25" s="47" t="s">
-        <v>116</v>
+        <v>449</v>
+      </c>
+      <c r="C25" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>117</v>
       </c>
       <c r="F25" s="30" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="K25" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="L25" s="103" t="s">
-        <v>450</v>
+        <v>446</v>
+      </c>
+      <c r="L25" s="104" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="30" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>452</v>
-      </c>
-      <c r="C26" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E26" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="F26" s="71" t="s">
-        <v>436</v>
-      </c>
-      <c r="G26" s="71" t="s">
         <v>453</v>
+      </c>
+      <c r="C26" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" s="72" t="s">
+        <v>437</v>
+      </c>
+      <c r="G26" s="72" t="s">
+        <v>454</v>
       </c>
       <c r="K26" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="L26" s="103" t="s">
-        <v>454</v>
+      <c r="L26" s="104" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="30" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>456</v>
-      </c>
-      <c r="C27" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="71" t="s">
-        <v>453</v>
-      </c>
-      <c r="G27" s="71" t="s">
         <v>457</v>
       </c>
+      <c r="C27" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F27" s="72" t="s">
+        <v>454</v>
+      </c>
+      <c r="G27" s="72" t="s">
+        <v>458</v>
+      </c>
       <c r="K27" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="L27" s="104">
+        <v>446</v>
+      </c>
+      <c r="L27" s="105">
         <v>244221.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="30" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>459</v>
-      </c>
-      <c r="C28" s="88" t="s">
-        <v>385</v>
-      </c>
-      <c r="E28" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="71" t="s">
-        <v>453</v>
-      </c>
-      <c r="G28" s="71" t="s">
         <v>460</v>
       </c>
+      <c r="C28" s="89" t="s">
+        <v>386</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="72" t="s">
+        <v>454</v>
+      </c>
+      <c r="G28" s="72" t="s">
+        <v>461</v>
+      </c>
       <c r="K28" s="30" t="s">
-        <v>445</v>
-      </c>
-      <c r="L28" s="105" t="s">
-        <v>461</v>
+        <v>446</v>
+      </c>
+      <c r="L28" s="106" t="s">
+        <v>462</v>
       </c>
     </row>
   </sheetData>
@@ -6822,20 +6829,20 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="79" t="s">
-        <v>462</v>
+      <c r="D1" s="80" t="s">
+        <v>463</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="2">
@@ -6870,26 +6877,26 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="106" t="s">
-        <v>343</v>
-      </c>
-      <c r="D1" s="106" t="s">
-        <v>464</v>
+      <c r="C1" s="107" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="107" t="s">
+        <v>465</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="G1" s="106" t="s">
-        <v>321</v>
+        <v>467</v>
+      </c>
+      <c r="G1" s="107" t="s">
+        <v>322</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
@@ -6897,72 +6904,72 @@
     </row>
     <row r="2">
       <c r="A2" s="18" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>467</v>
-      </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="108"/>
-      <c r="G2" s="108"/>
+        <v>468</v>
+      </c>
+      <c r="C2" s="108"/>
+      <c r="D2" s="109"/>
+      <c r="G2" s="109"/>
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>468</v>
-      </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="109"/>
-      <c r="G3" s="108"/>
+        <v>469</v>
+      </c>
+      <c r="C3" s="109"/>
+      <c r="D3" s="110"/>
+      <c r="G3" s="109"/>
     </row>
     <row r="4" ht="137.25" customHeight="1">
       <c r="A4" s="18" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="C4" s="108"/>
+        <v>470</v>
+      </c>
+      <c r="C4" s="109"/>
       <c r="D4" s="13"/>
-      <c r="E4" s="110"/>
-      <c r="G4" s="109"/>
+      <c r="E4" s="111"/>
+      <c r="G4" s="110"/>
     </row>
     <row r="5">
       <c r="A5" s="18" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>470</v>
-      </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
-      <c r="G5" s="109"/>
+        <v>471</v>
+      </c>
+      <c r="C5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
     </row>
     <row r="6" ht="120.75" customHeight="1">
       <c r="A6" s="18" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>471</v>
-      </c>
-      <c r="D6" s="111"/>
-      <c r="E6" s="112"/>
-      <c r="G6" s="108"/>
+        <v>472</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="113"/>
+      <c r="G6" s="109"/>
     </row>
     <row r="7" ht="120.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>472</v>
-      </c>
-      <c r="D7" s="111"/>
-      <c r="E7" s="112"/>
-      <c r="G7" s="108"/>
+        <v>473</v>
+      </c>
+      <c r="D7" s="112"/>
+      <c r="E7" s="113"/>
+      <c r="G7" s="109"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6986,16 +6993,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -7018,34 +7025,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="114"/>
-      <c r="C2" s="115"/>
+      <c r="A2" s="115"/>
+      <c r="C2" s="116"/>
     </row>
     <row r="3">
-      <c r="A3" s="116"/>
-      <c r="C3" s="115"/>
+      <c r="A3" s="117"/>
+      <c r="C3" s="116"/>
     </row>
     <row r="4">
-      <c r="A4" s="117"/>
-      <c r="C4" s="115"/>
+      <c r="A4" s="118"/>
+      <c r="C4" s="116"/>
     </row>
     <row r="5">
-      <c r="A5" s="117"/>
-      <c r="C5" s="115"/>
+      <c r="A5" s="118"/>
+      <c r="C5" s="116"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update models to latest version
</commit_message>
<xml_diff>
--- a/models/dev-layout-conn/source/dev-layout-conn.xlsx
+++ b/models/dev-layout-conn/source/dev-layout-conn.xlsx
@@ -295,7 +295,7 @@
     <t>223a</t>
   </si>
   <si>
-    <t>Aortis arch to demo wiredTo</t>
+    <t>Aortic arch to demo wiredTo</t>
   </si>
   <si>
     <t>Aortic arch</t>
@@ -820,7 +820,7 @@
     <t>Central nervous system tissue</t>
   </si>
   <si>
-    <t>UBERON:0001017</t>
+    <t>UBERON:0005158</t>
   </si>
   <si>
     <t>Aqueous solution</t>
@@ -1177,7 +1177,7 @@
     <t>ton-leaf-5</t>
   </si>
   <si>
-    <t>w-X-Z</t>
+    <t>w-Z-X</t>
   </si>
   <si>
     <t>oeso</t>
@@ -1189,7 +1189,7 @@
     <t>oeso-leaf-6</t>
   </si>
   <si>
-    <t>w-O-X</t>
+    <t>w-X-O</t>
   </si>
   <si>
     <t>IML1-SCG-d</t>
@@ -1598,7 +1598,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="27">
+  <fonts count="31">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1633,6 +1633,17 @@
       <name val="&quot;Helvetica Neue&quot;"/>
     </font>
     <font>
+      <strike/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <strike/>
+      <color rgb="FF555555"/>
+      <name val="&quot;Helvetica Neue&quot;"/>
+    </font>
+    <font>
+      <strike/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1657,6 +1668,9 @@
       <name val="&quot;docs-Helvetica Neue&quot;"/>
     </font>
     <font>
+      <name val="Arial"/>
+    </font>
+    <font>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
@@ -1673,6 +1687,11 @@
       <b/>
       <sz val="9.0"/>
       <color rgb="FF660E7A"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <strike/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -1720,7 +1739,7 @@
       <color rgb="FF1155CC"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1775,6 +1794,12 @@
         <bgColor rgb="FF3D85C6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -1796,7 +1821,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="143">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1911,6 +1936,28 @@
     <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1920,7 +1967,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1941,7 +1988,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1965,126 +2012,135 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="7" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="7" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
@@ -2097,22 +2153,25 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2124,25 +2183,28 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2160,31 +2222,31 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2496,7 +2558,7 @@
       <c r="A2" s="17" t="s">
         <v>492</v>
       </c>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="139" t="s">
         <v>493</v>
       </c>
     </row>
@@ -2504,7 +2566,7 @@
       <c r="A3" s="17" t="s">
         <v>494</v>
       </c>
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="140" t="s">
         <v>495</v>
       </c>
     </row>
@@ -2512,7 +2574,7 @@
       <c r="A4" s="17" t="s">
         <v>496</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="141" t="s">
         <v>497</v>
       </c>
     </row>
@@ -2520,7 +2582,7 @@
       <c r="A5" s="17" t="s">
         <v>498</v>
       </c>
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="141" t="s">
         <v>499</v>
       </c>
     </row>
@@ -2528,7 +2590,7 @@
       <c r="A6" s="17" t="s">
         <v>500</v>
       </c>
-      <c r="B6" s="128" t="s">
+      <c r="B6" s="141" t="s">
         <v>501</v>
       </c>
     </row>
@@ -2536,7 +2598,7 @@
       <c r="A7" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="B7" s="128" t="s">
+      <c r="B7" s="141" t="s">
         <v>503</v>
       </c>
     </row>
@@ -2544,7 +2606,7 @@
       <c r="A8" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="B8" s="128" t="s">
+      <c r="B8" s="141" t="s">
         <v>505</v>
       </c>
     </row>
@@ -2552,7 +2614,7 @@
       <c r="A9" s="17" t="s">
         <v>506</v>
       </c>
-      <c r="B9" s="128" t="s">
+      <c r="B9" s="141" t="s">
         <v>507</v>
       </c>
     </row>
@@ -2560,7 +2622,7 @@
       <c r="A10" s="17" t="s">
         <v>508</v>
       </c>
-      <c r="B10" s="128" t="s">
+      <c r="B10" s="141" t="s">
         <v>509</v>
       </c>
     </row>
@@ -2568,7 +2630,7 @@
       <c r="A11" s="17" t="s">
         <v>510</v>
       </c>
-      <c r="B11" s="128" t="s">
+      <c r="B11" s="141" t="s">
         <v>511</v>
       </c>
     </row>
@@ -2576,7 +2638,7 @@
       <c r="A12" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="B12" s="129" t="s">
+      <c r="B12" s="142" t="s">
         <v>513</v>
       </c>
     </row>
@@ -3320,27 +3382,30 @@
       <c r="B25" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="17"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="17"/>
-      <c r="T25" s="21"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="39"/>
+      <c r="O25" s="39"/>
+      <c r="P25" s="39"/>
+      <c r="Q25" s="44"/>
+      <c r="R25" s="39"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="45"/>
     </row>
     <row r="26">
       <c r="A26" s="14">
         <v>223.0</v>
       </c>
-      <c r="B26" s="38" t="s">
+      <c r="B26" s="46" t="s">
         <v>82</v>
       </c>
       <c r="C26" s="24" t="s">
@@ -3367,7 +3432,7 @@
       <c r="A27" s="14">
         <v>224.0</v>
       </c>
-      <c r="B27" s="39" t="s">
+      <c r="B27" s="47" t="s">
         <v>85</v>
       </c>
       <c r="C27" s="24" t="s">
@@ -3394,7 +3459,7 @@
       <c r="A28" s="14">
         <v>225.0</v>
       </c>
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="47" t="s">
         <v>88</v>
       </c>
       <c r="C28" s="24" t="s">
@@ -3421,7 +3486,7 @@
       <c r="A29" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="47" t="s">
         <v>92</v>
       </c>
       <c r="C29" s="24" t="s">
@@ -3432,10 +3497,10 @@
       <c r="F29" s="15"/>
       <c r="G29" s="17"/>
       <c r="I29" s="19"/>
-      <c r="J29" s="40">
+      <c r="J29" s="48">
         <v>110.0</v>
       </c>
-      <c r="M29" s="41">
+      <c r="M29" s="49">
         <v>254.0</v>
       </c>
       <c r="N29" s="25">
@@ -3451,7 +3516,7 @@
       <c r="A30" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B30" s="39" t="s">
+      <c r="B30" s="47" t="s">
         <v>95</v>
       </c>
       <c r="C30" s="24" t="s">
@@ -3462,10 +3527,10 @@
       <c r="F30" s="15"/>
       <c r="G30" s="17"/>
       <c r="I30" s="19"/>
-      <c r="J30" s="40">
+      <c r="J30" s="48">
         <v>110.0</v>
       </c>
-      <c r="M30" s="41">
+      <c r="M30" s="49">
         <v>255.0</v>
       </c>
       <c r="N30" s="25">
@@ -3481,7 +3546,7 @@
       <c r="A31" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="47" t="s">
         <v>98</v>
       </c>
       <c r="C31" s="24" t="s">
@@ -3492,10 +3557,10 @@
       <c r="F31" s="15"/>
       <c r="G31" s="17"/>
       <c r="I31" s="19"/>
-      <c r="J31" s="40">
+      <c r="J31" s="48">
         <v>110.0</v>
       </c>
-      <c r="M31" s="41">
+      <c r="M31" s="49">
         <v>256.0</v>
       </c>
       <c r="N31" s="25">
@@ -3511,7 +3576,7 @@
       <c r="A32" s="14">
         <v>226.0</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="50" t="s">
         <v>100</v>
       </c>
       <c r="C32" s="24" t="s">
@@ -3538,7 +3603,7 @@
       <c r="A33" s="14">
         <v>227.0</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="50" t="s">
         <v>103</v>
       </c>
       <c r="C33" s="24" t="s">
@@ -3548,7 +3613,7 @@
       <c r="E33" s="18"/>
       <c r="F33" s="15"/>
       <c r="G33" s="17"/>
-      <c r="I33" s="43" t="s">
+      <c r="I33" s="51" t="s">
         <v>105</v>
       </c>
       <c r="J33" s="17"/>
@@ -3580,7 +3645,7 @@
       <c r="M34" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="N34" s="44">
+      <c r="N34" s="52">
         <v>0.0</v>
       </c>
       <c r="O34" s="17"/>
@@ -3596,10 +3661,10 @@
       <c r="B35" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="45" t="s">
+      <c r="C35" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="E35" s="46" t="b">
+      <c r="E35" s="54" t="b">
         <v>1</v>
       </c>
       <c r="G35" s="17"/>
@@ -3617,16 +3682,16 @@
       <c r="T35" s="21"/>
     </row>
     <row r="36">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="55" t="s">
         <v>112</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="C36" s="48" t="s">
+      <c r="C36" s="56" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="49" t="b">
+      <c r="E36" s="57" t="b">
         <v>1</v>
       </c>
       <c r="F36" s="17" t="s">
@@ -3644,19 +3709,19 @@
       <c r="T36" s="21"/>
     </row>
     <row r="37">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="55" t="s">
         <v>115</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="48" t="s">
+      <c r="C37" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="49" t="b">
+      <c r="E37" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="F37" s="50" t="s">
+      <c r="F37" s="58" t="s">
         <v>114</v>
       </c>
       <c r="I37" s="19"/>
@@ -3671,19 +3736,19 @@
       <c r="T37" s="21"/>
     </row>
     <row r="38">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="55" t="s">
         <v>118</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="48" t="s">
+      <c r="C38" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="E38" s="49" t="b">
+      <c r="E38" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F38" s="58" t="s">
         <v>120</v>
       </c>
       <c r="I38" s="19"/>
@@ -3698,19 +3763,19 @@
       <c r="T38" s="21"/>
     </row>
     <row r="39">
-      <c r="A39" s="47" t="s">
+      <c r="A39" s="55" t="s">
         <v>121</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="48" t="s">
+      <c r="C39" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="49" t="b">
+      <c r="E39" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="F39" s="50" t="s">
+      <c r="F39" s="58" t="s">
         <v>114</v>
       </c>
       <c r="I39" s="19"/>
@@ -3725,19 +3790,19 @@
       <c r="T39" s="21"/>
     </row>
     <row r="40">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="55" t="s">
         <v>124</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="C40" s="48" t="s">
+      <c r="C40" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="E40" s="49" t="b">
+      <c r="E40" s="57" t="b">
         <v>1</v>
       </c>
-      <c r="F40" s="50" t="s">
+      <c r="F40" s="58" t="s">
         <v>120</v>
       </c>
       <c r="I40" s="19"/>
@@ -3758,7 +3823,7 @@
       <c r="B41" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="C41" s="45" t="s">
+      <c r="C41" s="53" t="s">
         <v>128</v>
       </c>
       <c r="D41" s="17"/>
@@ -3766,10 +3831,10 @@
       <c r="F41" s="15"/>
       <c r="G41" s="17"/>
       <c r="I41" s="19"/>
-      <c r="J41" s="40">
+      <c r="J41" s="48">
         <v>107.0</v>
       </c>
-      <c r="M41" s="51">
+      <c r="M41" s="59">
         <v>228.0</v>
       </c>
       <c r="N41" s="25">
@@ -3788,7 +3853,7 @@
       <c r="B42" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="45" t="s">
+      <c r="C42" s="53" t="s">
         <v>131</v>
       </c>
       <c r="D42" s="17"/>
@@ -3796,10 +3861,10 @@
       <c r="F42" s="15"/>
       <c r="G42" s="17"/>
       <c r="I42" s="19"/>
-      <c r="J42" s="40">
+      <c r="J42" s="48">
         <v>107.0</v>
       </c>
-      <c r="M42" s="40">
+      <c r="M42" s="48">
         <v>201.0</v>
       </c>
       <c r="N42" s="25">
@@ -3815,10 +3880,10 @@
       <c r="A43" s="14">
         <v>230.0</v>
       </c>
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="60" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="45" t="s">
+      <c r="C43" s="53" t="s">
         <v>133</v>
       </c>
       <c r="D43" s="17"/>
@@ -3842,10 +3907,10 @@
       <c r="A44" s="14">
         <v>231.0</v>
       </c>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="53" t="s">
         <v>135</v>
       </c>
       <c r="D44" s="17"/>
@@ -3869,10 +3934,10 @@
       <c r="A45" s="14">
         <v>232.0</v>
       </c>
-      <c r="B45" s="52" t="s">
+      <c r="B45" s="60" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="45" t="s">
+      <c r="C45" s="53" t="s">
         <v>137</v>
       </c>
       <c r="D45" s="17"/>
@@ -3896,10 +3961,10 @@
       <c r="A46" s="14">
         <v>233.0</v>
       </c>
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="53" t="s">
         <v>139</v>
       </c>
       <c r="D46" s="17"/>
@@ -3922,20 +3987,20 @@
       <c r="A47" s="14">
         <v>234.0</v>
       </c>
-      <c r="B47" s="52" t="s">
+      <c r="B47" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="45" t="s">
+      <c r="C47" s="53" t="s">
         <v>141</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="18"/>
       <c r="F47" s="15"/>
       <c r="G47" s="17"/>
-      <c r="I47" s="53">
+      <c r="I47" s="61">
         <v>117.0</v>
       </c>
-      <c r="J47" s="54"/>
+      <c r="J47" s="62"/>
       <c r="L47" s="17"/>
       <c r="M47" s="15"/>
       <c r="N47" s="17"/>
@@ -3949,13 +4014,13 @@
       <c r="A48" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="B48" s="52" t="s">
+      <c r="B48" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="55" t="s">
+      <c r="C48" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="E48" s="46" t="b">
+      <c r="E48" s="54" t="b">
         <v>1</v>
       </c>
       <c r="F48" s="17" t="s">
@@ -3977,10 +4042,10 @@
       <c r="A49" s="14">
         <v>235.0</v>
       </c>
-      <c r="B49" s="52" t="s">
+      <c r="B49" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="C49" s="45" t="s">
+      <c r="C49" s="53" t="s">
         <v>146</v>
       </c>
       <c r="D49" s="17"/>
@@ -4004,10 +4069,10 @@
       <c r="A50" s="14">
         <v>236.0</v>
       </c>
-      <c r="B50" s="52" t="s">
+      <c r="B50" s="60" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="45" t="s">
+      <c r="C50" s="53" t="s">
         <v>148</v>
       </c>
       <c r="D50" s="17"/>
@@ -4031,7 +4096,7 @@
       <c r="A51" s="14">
         <v>237.0</v>
       </c>
-      <c r="B51" s="52" t="s">
+      <c r="B51" s="60" t="s">
         <v>149</v>
       </c>
       <c r="C51" s="24" t="s">
@@ -4058,7 +4123,7 @@
       <c r="A52" s="14">
         <v>238.0</v>
       </c>
-      <c r="B52" s="52" t="s">
+      <c r="B52" s="60" t="s">
         <v>151</v>
       </c>
       <c r="C52" s="24" t="s">
@@ -4085,7 +4150,7 @@
       <c r="A53" s="14">
         <v>239.0</v>
       </c>
-      <c r="B53" s="52" t="s">
+      <c r="B53" s="60" t="s">
         <v>153</v>
       </c>
       <c r="C53" s="24" t="s">
@@ -4099,7 +4164,7 @@
         <v>117.0</v>
       </c>
       <c r="J53" s="17"/>
-      <c r="M53" s="40">
+      <c r="M53" s="48">
         <v>249.0</v>
       </c>
       <c r="N53" s="25">
@@ -4129,7 +4194,7 @@
         <v>117.0</v>
       </c>
       <c r="J54" s="17"/>
-      <c r="M54" s="40">
+      <c r="M54" s="48">
         <v>248.0</v>
       </c>
       <c r="N54" s="25">
@@ -4168,7 +4233,7 @@
       <c r="T55" s="17"/>
     </row>
     <row r="56">
-      <c r="A56" s="56" t="s">
+      <c r="A56" s="64" t="s">
         <v>159</v>
       </c>
       <c r="B56" s="12" t="s">
@@ -4182,7 +4247,7 @@
       <c r="F56" s="15"/>
       <c r="G56" s="17"/>
       <c r="I56" s="19"/>
-      <c r="J56" s="40">
+      <c r="J56" s="48">
         <v>114.0</v>
       </c>
       <c r="M56" s="14">
@@ -4198,7 +4263,7 @@
       <c r="T56" s="17"/>
     </row>
     <row r="57">
-      <c r="A57" s="56" t="s">
+      <c r="A57" s="64" t="s">
         <v>162</v>
       </c>
       <c r="B57" s="12" t="s">
@@ -4212,11 +4277,11 @@
       <c r="F57" s="15"/>
       <c r="G57" s="17"/>
       <c r="I57" s="19"/>
-      <c r="J57" s="40">
+      <c r="J57" s="48">
         <v>112.0</v>
       </c>
       <c r="L57" s="15"/>
-      <c r="M57" s="57"/>
+      <c r="M57" s="65"/>
       <c r="N57" s="15"/>
       <c r="O57" s="17"/>
       <c r="P57" s="17"/>
@@ -4225,10 +4290,10 @@
       <c r="T57" s="17"/>
     </row>
     <row r="58">
-      <c r="A58" s="58">
+      <c r="A58" s="66">
         <v>242.0</v>
       </c>
-      <c r="B58" s="52" t="s">
+      <c r="B58" s="60" t="s">
         <v>165</v>
       </c>
       <c r="C58" s="24" t="s">
@@ -4252,10 +4317,10 @@
       <c r="T58" s="17"/>
     </row>
     <row r="59">
-      <c r="A59" s="58">
+      <c r="A59" s="66">
         <v>243.0</v>
       </c>
-      <c r="B59" s="52" t="s">
+      <c r="B59" s="60" t="s">
         <v>167</v>
       </c>
       <c r="C59" s="24" t="s">
@@ -4279,10 +4344,10 @@
       <c r="T59" s="21"/>
     </row>
     <row r="60">
-      <c r="A60" s="58">
+      <c r="A60" s="66">
         <v>244.0</v>
       </c>
-      <c r="B60" s="52" t="s">
+      <c r="B60" s="60" t="s">
         <v>169</v>
       </c>
       <c r="C60" s="24" t="s">
@@ -4304,10 +4369,10 @@
       <c r="T60" s="21"/>
     </row>
     <row r="61">
-      <c r="A61" s="59">
+      <c r="A61" s="67">
         <v>245.0</v>
       </c>
-      <c r="B61" s="52" t="s">
+      <c r="B61" s="60" t="s">
         <v>171</v>
       </c>
       <c r="C61" s="24" t="s">
@@ -4329,13 +4394,13 @@
       <c r="T61" s="21"/>
     </row>
     <row r="62">
-      <c r="A62" s="59">
+      <c r="A62" s="67">
         <v>246.0</v>
       </c>
-      <c r="B62" s="52" t="s">
+      <c r="B62" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="60" t="s">
+      <c r="C62" s="68" t="s">
         <v>174</v>
       </c>
       <c r="D62" s="17"/>
@@ -4354,13 +4419,13 @@
       <c r="T62" s="21"/>
     </row>
     <row r="63">
-      <c r="A63" s="59">
+      <c r="A63" s="67">
         <v>247.0</v>
       </c>
-      <c r="B63" s="52" t="s">
+      <c r="B63" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="60" t="s">
+      <c r="C63" s="68" t="s">
         <v>176</v>
       </c>
       <c r="D63" s="17"/>
@@ -4379,13 +4444,13 @@
       <c r="T63" s="21"/>
     </row>
     <row r="64">
-      <c r="A64" s="59">
+      <c r="A64" s="67">
         <v>248.0</v>
       </c>
-      <c r="B64" s="52" t="s">
+      <c r="B64" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="C64" s="60" t="s">
+      <c r="C64" s="68" t="s">
         <v>178</v>
       </c>
       <c r="D64" s="17"/>
@@ -4394,7 +4459,7 @@
       <c r="G64" s="17"/>
       <c r="I64" s="19"/>
       <c r="J64" s="15"/>
-      <c r="L64" s="61"/>
+      <c r="L64" s="69"/>
       <c r="M64" s="17"/>
       <c r="N64" s="17"/>
       <c r="O64" s="17"/>
@@ -4404,13 +4469,13 @@
       <c r="T64" s="21"/>
     </row>
     <row r="65">
-      <c r="A65" s="59">
+      <c r="A65" s="67">
         <v>249.0</v>
       </c>
-      <c r="B65" s="52" t="s">
+      <c r="B65" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="C65" s="60" t="s">
+      <c r="C65" s="68" t="s">
         <v>180</v>
       </c>
       <c r="D65" s="17"/>
@@ -4418,8 +4483,8 @@
       <c r="F65" s="15"/>
       <c r="G65" s="17"/>
       <c r="I65" s="19"/>
-      <c r="J65" s="62"/>
-      <c r="M65" s="63" t="s">
+      <c r="J65" s="70"/>
+      <c r="M65" s="71" t="s">
         <v>181</v>
       </c>
       <c r="N65" s="25">
@@ -4432,13 +4497,13 @@
       <c r="T65" s="21"/>
     </row>
     <row r="66">
-      <c r="A66" s="59">
+      <c r="A66" s="67">
         <v>250.0</v>
       </c>
-      <c r="B66" s="52" t="s">
+      <c r="B66" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C66" s="60" t="s">
+      <c r="C66" s="68" t="s">
         <v>183</v>
       </c>
       <c r="D66" s="17"/>
@@ -4457,13 +4522,13 @@
       <c r="T66" s="21"/>
     </row>
     <row r="67">
-      <c r="A67" s="59">
+      <c r="A67" s="67">
         <v>251.0</v>
       </c>
-      <c r="B67" s="52" t="s">
+      <c r="B67" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="C67" s="60" t="s">
+      <c r="C67" s="68" t="s">
         <v>185</v>
       </c>
       <c r="D67" s="17"/>
@@ -4482,13 +4547,13 @@
       <c r="T67" s="21"/>
     </row>
     <row r="68">
-      <c r="A68" s="59">
+      <c r="A68" s="67">
         <v>252.0</v>
       </c>
-      <c r="B68" s="52" t="s">
+      <c r="B68" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="60" t="s">
+      <c r="C68" s="68" t="s">
         <v>187</v>
       </c>
       <c r="D68" s="17"/>
@@ -4507,13 +4572,13 @@
       <c r="T68" s="21"/>
     </row>
     <row r="69">
-      <c r="A69" s="59">
+      <c r="A69" s="67">
         <v>253.0</v>
       </c>
-      <c r="B69" s="52" t="s">
+      <c r="B69" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="C69" s="60" t="s">
+      <c r="C69" s="68" t="s">
         <v>189</v>
       </c>
       <c r="D69" s="17"/>
@@ -4532,13 +4597,13 @@
       <c r="T69" s="21"/>
     </row>
     <row r="70">
-      <c r="A70" s="59">
+      <c r="A70" s="67">
         <v>254.0</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C70" s="60" t="s">
+      <c r="C70" s="68" t="s">
         <v>191</v>
       </c>
       <c r="D70" s="17"/>
@@ -4557,13 +4622,13 @@
       <c r="T70" s="21"/>
     </row>
     <row r="71">
-      <c r="A71" s="59">
+      <c r="A71" s="67">
         <v>255.0</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C71" s="64" t="s">
+      <c r="C71" s="72" t="s">
         <v>193</v>
       </c>
       <c r="D71" s="17"/>
@@ -4582,7 +4647,7 @@
       <c r="T71" s="21"/>
     </row>
     <row r="72">
-      <c r="A72" s="59">
+      <c r="A72" s="67">
         <v>256.0</v>
       </c>
       <c r="B72" s="12" t="s">
@@ -4607,13 +4672,13 @@
       <c r="T72" s="21"/>
     </row>
     <row r="73">
-      <c r="A73" s="59">
+      <c r="A73" s="67">
         <v>257.0</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="60" t="s">
+      <c r="C73" s="68" t="s">
         <v>197</v>
       </c>
       <c r="D73" s="17"/>
@@ -4632,13 +4697,13 @@
       <c r="T73" s="21"/>
     </row>
     <row r="74">
-      <c r="A74" s="59">
+      <c r="A74" s="67">
         <v>258.0</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C74" s="60" t="s">
+      <c r="C74" s="68" t="s">
         <v>199</v>
       </c>
       <c r="D74" s="17"/>
@@ -4657,13 +4722,13 @@
       <c r="T74" s="21"/>
     </row>
     <row r="75">
-      <c r="A75" s="59">
+      <c r="A75" s="67">
         <v>259.0</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C75" s="65" t="s">
+      <c r="C75" s="73" t="s">
         <v>201</v>
       </c>
       <c r="D75" s="17"/>
@@ -4682,10 +4747,10 @@
       <c r="T75" s="21"/>
     </row>
     <row r="76">
-      <c r="A76" s="59">
+      <c r="A76" s="67">
         <v>260.0</v>
       </c>
-      <c r="B76" s="66" t="s">
+      <c r="B76" s="74" t="s">
         <v>202</v>
       </c>
       <c r="C76" s="24" t="s">
@@ -4704,14 +4769,14 @@
       <c r="P76" s="20"/>
       <c r="Q76" s="17"/>
       <c r="R76" s="21"/>
-      <c r="S76" s="67"/>
+      <c r="S76" s="75"/>
       <c r="T76" s="21"/>
     </row>
     <row r="77">
-      <c r="A77" s="59">
+      <c r="A77" s="67">
         <v>261.0</v>
       </c>
-      <c r="B77" s="66" t="s">
+      <c r="B77" s="74" t="s">
         <v>204</v>
       </c>
       <c r="C77" s="16" t="s">
@@ -4730,17 +4795,17 @@
       <c r="P77" s="20"/>
       <c r="Q77" s="17"/>
       <c r="R77" s="21"/>
-      <c r="S77" s="67"/>
+      <c r="S77" s="75"/>
       <c r="T77" s="21"/>
     </row>
     <row r="78">
-      <c r="A78" s="68" t="s">
+      <c r="A78" s="76" t="s">
         <v>206</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="60" t="s">
+      <c r="C78" s="68" t="s">
         <v>208</v>
       </c>
       <c r="D78" s="17"/>
@@ -4764,13 +4829,13 @@
       <c r="T78" s="21"/>
     </row>
     <row r="79">
-      <c r="A79" s="68" t="s">
+      <c r="A79" s="76" t="s">
         <v>211</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="60" t="s">
+      <c r="C79" s="68" t="s">
         <v>213</v>
       </c>
       <c r="D79" s="17"/>
@@ -4794,13 +4859,13 @@
       <c r="T79" s="21"/>
     </row>
     <row r="80">
-      <c r="A80" s="68" t="s">
+      <c r="A80" s="76" t="s">
         <v>214</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C80" s="60" t="s">
+      <c r="C80" s="68" t="s">
         <v>216</v>
       </c>
       <c r="D80" s="17"/>
@@ -4824,13 +4889,13 @@
       <c r="T80" s="21"/>
     </row>
     <row r="81">
-      <c r="A81" s="59">
+      <c r="A81" s="67">
         <v>262.0</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C81" s="60" t="s">
+      <c r="C81" s="68" t="s">
         <v>218</v>
       </c>
       <c r="D81" s="17"/>
@@ -4850,13 +4915,13 @@
       <c r="T81" s="21"/>
     </row>
     <row r="82">
-      <c r="A82" s="59">
+      <c r="A82" s="67">
         <v>263.0</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C82" s="60" t="s">
+      <c r="C82" s="68" t="s">
         <v>220</v>
       </c>
       <c r="D82" s="17"/>
@@ -4876,13 +4941,13 @@
       <c r="T82" s="21"/>
     </row>
     <row r="83">
-      <c r="A83" s="59">
+      <c r="A83" s="67">
         <v>264.0</v>
       </c>
       <c r="B83" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C83" s="60" t="s">
+      <c r="C83" s="68" t="s">
         <v>222</v>
       </c>
       <c r="D83" s="17"/>
@@ -4902,13 +4967,13 @@
       <c r="T83" s="21"/>
     </row>
     <row r="84">
-      <c r="A84" s="59">
+      <c r="A84" s="67">
         <v>265.0</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C84" s="60" t="s">
+      <c r="C84" s="68" t="s">
         <v>224</v>
       </c>
       <c r="D84" s="17"/>
@@ -4917,7 +4982,7 @@
       <c r="G84" s="17"/>
       <c r="I84" s="19"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="69"/>
+      <c r="K84" s="77"/>
       <c r="M84" s="26" t="s">
         <v>225</v>
       </c>
@@ -4931,13 +4996,13 @@
       <c r="T84" s="21"/>
     </row>
     <row r="85">
-      <c r="A85" s="59">
+      <c r="A85" s="67">
         <v>266.0</v>
       </c>
       <c r="B85" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C85" s="60" t="s">
+      <c r="C85" s="68" t="s">
         <v>227</v>
       </c>
       <c r="D85" s="17"/>
@@ -4946,7 +5011,7 @@
       <c r="G85" s="17"/>
       <c r="I85" s="19"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="69"/>
+      <c r="K85" s="77"/>
       <c r="M85" s="26" t="s">
         <v>228</v>
       </c>
@@ -4960,13 +5025,13 @@
       <c r="T85" s="21"/>
     </row>
     <row r="86">
-      <c r="A86" s="68" t="s">
+      <c r="A86" s="76" t="s">
         <v>229</v>
       </c>
       <c r="B86" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C86" s="60" t="s">
+      <c r="C86" s="68" t="s">
         <v>231</v>
       </c>
       <c r="D86" s="17"/>
@@ -4977,7 +5042,7 @@
       <c r="J86" s="14">
         <v>108.0</v>
       </c>
-      <c r="K86" s="69"/>
+      <c r="K86" s="77"/>
       <c r="M86" s="14">
         <v>257.0</v>
       </c>
@@ -4991,13 +5056,13 @@
       <c r="T86" s="21"/>
     </row>
     <row r="87">
-      <c r="A87" s="68" t="s">
+      <c r="A87" s="76" t="s">
         <v>232</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="C87" s="60" t="s">
+      <c r="C87" s="68" t="s">
         <v>234</v>
       </c>
       <c r="D87" s="17"/>
@@ -5008,7 +5073,7 @@
       <c r="J87" s="14">
         <v>109.0</v>
       </c>
-      <c r="K87" s="69"/>
+      <c r="K87" s="77"/>
       <c r="L87" s="15"/>
       <c r="M87" s="15"/>
       <c r="N87" s="17"/>
@@ -5025,7 +5090,7 @@
       <c r="B88" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C88" s="70" t="s">
+      <c r="C88" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D88" s="17"/>
@@ -5036,7 +5101,7 @@
       <c r="J88" s="14">
         <v>229.0</v>
       </c>
-      <c r="K88" s="69"/>
+      <c r="K88" s="77"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
       <c r="N88" s="17"/>
@@ -5055,7 +5120,7 @@
       <c r="B89" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="C89" s="70" t="s">
+      <c r="C89" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D89" s="17"/>
@@ -5066,7 +5131,7 @@
       <c r="J89" s="14">
         <v>229.0</v>
       </c>
-      <c r="K89" s="69"/>
+      <c r="K89" s="77"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
       <c r="N89" s="17"/>
@@ -5085,7 +5150,7 @@
       <c r="B90" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C90" s="70" t="s">
+      <c r="C90" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D90" s="17"/>
@@ -5096,7 +5161,7 @@
       <c r="J90" s="14">
         <v>229.0</v>
       </c>
-      <c r="K90" s="69"/>
+      <c r="K90" s="77"/>
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
       <c r="N90" s="17"/>
@@ -5115,7 +5180,7 @@
       <c r="B91" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="C91" s="70" t="s">
+      <c r="C91" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D91" s="17"/>
@@ -5124,10 +5189,10 @@
       <c r="G91" s="17"/>
       <c r="H91" s="17"/>
       <c r="I91" s="19"/>
-      <c r="J91" s="40">
+      <c r="J91" s="48">
         <v>229.0</v>
       </c>
-      <c r="K91" s="38"/>
+      <c r="K91" s="46"/>
       <c r="L91" s="17"/>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
@@ -5145,7 +5210,7 @@
       <c r="B92" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C92" s="70" t="s">
+      <c r="C92" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D92" s="17"/>
@@ -5156,7 +5221,7 @@
       <c r="J92" s="14">
         <v>229.0</v>
       </c>
-      <c r="K92" s="69"/>
+      <c r="K92" s="77"/>
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
       <c r="N92" s="17"/>
@@ -5176,7 +5241,7 @@
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A93,1),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (4) (bolew)</v>
       </c>
-      <c r="C93" s="70" t="s">
+      <c r="C93" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D93" s="17"/>
@@ -5187,7 +5252,7 @@
       <c r="J93" s="14">
         <v>229.0</v>
       </c>
-      <c r="K93" s="69"/>
+      <c r="K93" s="77"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
       <c r="N93" s="17"/>
@@ -5207,7 +5272,7 @@
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A94,2),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (10) (bolew)</v>
       </c>
-      <c r="C94" s="70" t="s">
+      <c r="C94" s="78" t="s">
         <v>236</v>
       </c>
       <c r="D94" s="17"/>
@@ -5218,7 +5283,7 @@
       <c r="J94" s="14">
         <v>229.0</v>
       </c>
-      <c r="K94" s="69"/>
+      <c r="K94" s="77"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15"/>
       <c r="N94" s="17"/>
@@ -5231,22 +5296,22 @@
       <c r="T94" s="21"/>
     </row>
     <row r="95">
-      <c r="A95" s="71" t="s">
+      <c r="A95" s="79" t="s">
         <v>249</v>
       </c>
-      <c r="B95" s="72" t="s">
+      <c r="B95" s="80" t="s">
         <v>250</v>
       </c>
-      <c r="C95" s="70"/>
+      <c r="C95" s="78"/>
       <c r="D95" s="17"/>
       <c r="E95" s="18"/>
       <c r="F95" s="15"/>
       <c r="G95" s="17"/>
       <c r="I95" s="19"/>
       <c r="J95" s="14"/>
-      <c r="K95" s="69"/>
-      <c r="M95" s="73"/>
-      <c r="N95" s="73"/>
+      <c r="K95" s="77"/>
+      <c r="M95" s="81"/>
+      <c r="N95" s="81"/>
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
       <c r="Q95" s="20"/>
@@ -5269,22 +5334,22 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.86"/>
+    <col customWidth="1" min="2" max="2" width="31.71"/>
     <col customWidth="1" min="3" max="3" width="26.29"/>
     <col customWidth="1" min="4" max="4" width="28.86"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74" t="s">
+      <c r="B1" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="82" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5295,10 +5360,10 @@
       <c r="B2" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="C2" s="84" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="77"/>
+      <c r="D2" s="85"/>
     </row>
     <row r="3">
       <c r="A3" s="14">
@@ -5310,7 +5375,7 @@
       <c r="C3" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="D3" s="77"/>
+      <c r="D3" s="85"/>
     </row>
     <row r="4">
       <c r="A4" s="14">
@@ -5319,10 +5384,10 @@
       <c r="B4" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5">
       <c r="A5" s="14">
@@ -5334,7 +5399,7 @@
       <c r="C5" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="87" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5357,7 +5422,7 @@
       <c r="B7" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="88" t="s">
         <v>263</v>
       </c>
       <c r="D7" s="17"/>
@@ -5369,7 +5434,7 @@
       <c r="B8" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="88" t="s">
         <v>265</v>
       </c>
       <c r="D8" s="17"/>
@@ -5381,7 +5446,7 @@
       <c r="B9" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="88" t="s">
         <v>267</v>
       </c>
       <c r="D9" s="17"/>
@@ -5432,7 +5497,7 @@
       <c r="C13" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="48">
         <v>53.0</v>
       </c>
     </row>
@@ -5458,7 +5523,7 @@
       <c r="C15" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="48">
         <v>55.0</v>
       </c>
     </row>
@@ -5481,7 +5546,7 @@
       <c r="B17" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="89" t="s">
         <v>283</v>
       </c>
       <c r="D17" s="17"/>
@@ -5493,7 +5558,7 @@
       <c r="B18" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="53" t="s">
         <v>285</v>
       </c>
       <c r="D18" s="17"/>
@@ -5505,10 +5570,10 @@
       <c r="B19" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="53" t="s">
         <v>287</v>
       </c>
-      <c r="D19" s="40">
+      <c r="D19" s="48">
         <v>53.0</v>
       </c>
     </row>
@@ -5519,10 +5584,10 @@
       <c r="B20" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="56" t="s">
         <v>289</v>
       </c>
-      <c r="D20" s="40"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21">
       <c r="A21" s="14">
@@ -5534,7 +5599,7 @@
       <c r="C21" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="D21" s="40">
+      <c r="D21" s="48">
         <v>100.0</v>
       </c>
     </row>
@@ -5545,10 +5610,10 @@
       <c r="B22" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="C22" s="48" t="s">
+      <c r="C22" s="56" t="s">
         <v>258</v>
       </c>
-      <c r="D22" s="40">
+      <c r="D22" s="48">
         <v>100.0</v>
       </c>
     </row>
@@ -5562,7 +5627,7 @@
       <c r="C23" s="12" t="s">
         <v>294</v>
       </c>
-      <c r="D23" s="40">
+      <c r="D23" s="48">
         <v>101.0</v>
       </c>
     </row>
@@ -5576,7 +5641,7 @@
       <c r="C24" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="48">
         <v>111.0</v>
       </c>
     </row>
@@ -5590,7 +5655,7 @@
       <c r="C25" s="16" t="s">
         <v>297</v>
       </c>
-      <c r="D25" s="40">
+      <c r="D25" s="48">
         <v>111.0</v>
       </c>
     </row>
@@ -5604,7 +5669,7 @@
       <c r="C26" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="D26" s="40">
+      <c r="D26" s="48">
         <v>111.0</v>
       </c>
     </row>
@@ -5618,7 +5683,7 @@
       <c r="C27" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="D27" s="40">
+      <c r="D27" s="48">
         <v>111.0</v>
       </c>
     </row>
@@ -5692,7 +5757,7 @@
       <c r="C33" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="D33" s="40">
+      <c r="D33" s="48">
         <v>53.0</v>
       </c>
     </row>
@@ -5706,7 +5771,7 @@
       <c r="C34" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="D34" s="40">
+      <c r="D34" s="48">
         <v>116.0</v>
       </c>
     </row>
@@ -5734,28 +5799,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="90" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="90" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="90" t="s">
         <v>316</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="H1" s="82" t="s">
+      <c r="H1" s="91" t="s">
         <v>318</v>
       </c>
     </row>
@@ -5811,7 +5876,7 @@
       <c r="H4" s="21"/>
     </row>
     <row r="5">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="79" t="s">
         <v>328</v>
       </c>
       <c r="B5" s="15"/>
@@ -5916,49 +5981,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="90" t="s">
         <v>340</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="90" t="s">
         <v>341</v>
       </c>
-      <c r="F1" s="83" t="s">
+      <c r="F1" s="92" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="90" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="90" t="s">
         <v>344</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="93" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="81" t="s">
+      <c r="K1" s="90" t="s">
         <v>346</v>
       </c>
-      <c r="L1" s="85" t="s">
+      <c r="L1" s="94" t="s">
         <v>347</v>
       </c>
-      <c r="M1" s="82" t="s">
+      <c r="M1" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="N1" s="82" t="s">
+      <c r="N1" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="82" t="s">
+      <c r="O1" s="91" t="s">
         <v>318</v>
       </c>
       <c r="P1" s="13" t="s">
@@ -5966,32 +6031,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="95" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87" t="s">
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="88"/>
-      <c r="F2" s="89" t="s">
+      <c r="E2" s="97"/>
+      <c r="F2" s="98" t="s">
         <v>350</v>
       </c>
-      <c r="G2" s="72" t="s">
+      <c r="G2" s="99" t="s">
         <v>351</v>
       </c>
-      <c r="H2" s="90"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="72" t="s">
+      <c r="H2" s="100"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="99" t="s">
         <v>352</v>
       </c>
-      <c r="P2" s="13"/>
+      <c r="P2" s="99"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
@@ -5999,17 +6064,17 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="91" t="s">
+      <c r="D3" s="101" t="s">
         <v>354</v>
       </c>
       <c r="E3" s="21"/>
-      <c r="F3" s="92" t="s">
+      <c r="F3" s="102" t="s">
         <v>355</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="90"/>
+      <c r="H3" s="103"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
@@ -6032,13 +6097,13 @@
         <v>359</v>
       </c>
       <c r="E4" s="21"/>
-      <c r="F4" s="92" t="s">
+      <c r="F4" s="102" t="s">
         <v>360</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="90"/>
+      <c r="H4" s="103"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
@@ -6057,18 +6122,18 @@
         <v>363</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="104" t="s">
         <v>364</v>
       </c>
-      <c r="E5" s="47"/>
-      <c r="F5" s="94" t="s">
+      <c r="E5" s="55"/>
+      <c r="F5" s="105" t="s">
         <v>365</v>
       </c>
-      <c r="G5" s="94" t="s">
+      <c r="G5" s="105" t="s">
         <v>366</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="47"/>
+      <c r="I5" s="55"/>
       <c r="J5" s="15"/>
       <c r="K5" s="2"/>
       <c r="L5" s="17"/>
@@ -6082,25 +6147,25 @@
         <v>367</v>
       </c>
       <c r="B6" s="15"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="96" t="s">
+      <c r="C6" s="106"/>
+      <c r="D6" s="107" t="s">
         <v>368</v>
       </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="94" t="s">
+      <c r="E6" s="55"/>
+      <c r="F6" s="105" t="s">
         <v>369</v>
       </c>
-      <c r="G6" s="94" t="s">
+      <c r="G6" s="105" t="s">
         <v>370</v>
       </c>
       <c r="H6" s="15"/>
-      <c r="I6" s="47"/>
+      <c r="I6" s="55"/>
       <c r="J6" s="15"/>
       <c r="K6" s="2"/>
       <c r="L6" s="17"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="72" t="s">
+      <c r="O6" s="80" t="s">
         <v>371</v>
       </c>
       <c r="P6" s="13" t="b">
@@ -6112,25 +6177,25 @@
         <v>372</v>
       </c>
       <c r="B7" s="15"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="97">
+      <c r="C7" s="106"/>
+      <c r="D7" s="108">
         <v>227.0</v>
       </c>
-      <c r="E7" s="47"/>
-      <c r="F7" s="94" t="s">
+      <c r="E7" s="55"/>
+      <c r="F7" s="105" t="s">
         <v>373</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="105" t="s">
         <v>374</v>
       </c>
       <c r="H7" s="15"/>
-      <c r="I7" s="47"/>
+      <c r="I7" s="55"/>
       <c r="J7" s="15"/>
       <c r="K7" s="2"/>
       <c r="L7" s="17"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="80" t="s">
         <v>375</v>
       </c>
       <c r="P7" s="13" t="b">
@@ -6142,25 +6207,25 @@
         <v>376</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="97">
+      <c r="C8" s="106"/>
+      <c r="D8" s="108">
         <v>259.0</v>
       </c>
-      <c r="E8" s="47"/>
-      <c r="F8" s="94" t="s">
+      <c r="E8" s="55"/>
+      <c r="F8" s="105" t="s">
         <v>377</v>
       </c>
-      <c r="G8" s="94" t="s">
+      <c r="G8" s="105" t="s">
         <v>378</v>
       </c>
       <c r="H8" s="15"/>
-      <c r="I8" s="47"/>
+      <c r="I8" s="55"/>
       <c r="J8" s="15"/>
       <c r="K8" s="2"/>
       <c r="L8" s="17"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="72" t="s">
+      <c r="O8" s="80" t="s">
         <v>379</v>
       </c>
       <c r="P8" s="13" t="b">
@@ -6174,21 +6239,21 @@
       <c r="B9" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="D9" s="98"/>
-      <c r="E9" s="47" t="s">
+      <c r="D9" s="109"/>
+      <c r="E9" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="99" t="s">
+      <c r="F9" s="110" t="s">
         <v>323</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="105" t="s">
         <v>383</v>
       </c>
       <c r="H9" s="15"/>
-      <c r="I9" s="47"/>
+      <c r="I9" s="55"/>
       <c r="J9" s="15"/>
       <c r="K9" s="2">
         <v>0.0</v>
@@ -6208,26 +6273,26 @@
       <c r="B10" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="C10" s="95" t="s">
+      <c r="C10" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="D10" s="98"/>
-      <c r="E10" s="47" t="s">
+      <c r="D10" s="109"/>
+      <c r="E10" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="99" t="s">
+      <c r="F10" s="110" t="s">
         <v>324</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="111" t="s">
         <v>387</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="100"/>
+      <c r="I10" s="112"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="101" t="s">
+      <c r="K10" s="113" t="s">
         <v>388</v>
       </c>
-      <c r="L10" s="100" t="s">
+      <c r="L10" s="112" t="s">
         <v>389</v>
       </c>
       <c r="M10" s="21"/>
@@ -6242,17 +6307,17 @@
       <c r="B11" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="D11" s="102"/>
-      <c r="E11" s="47" t="s">
+      <c r="D11" s="114"/>
+      <c r="E11" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="114" t="s">
         <v>326</v>
       </c>
-      <c r="G11" s="103" t="s">
+      <c r="G11" s="115" t="s">
         <v>392</v>
       </c>
       <c r="H11" s="15"/>
@@ -6260,7 +6325,7 @@
       <c r="K11" s="13">
         <v>0.0</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="49">
         <v>265.0</v>
       </c>
       <c r="M11" s="21"/>
@@ -6275,14 +6340,14 @@
       <c r="B12" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="47" t="s">
+      <c r="D12" s="110"/>
+      <c r="E12" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="99" t="s">
+      <c r="F12" s="110" t="s">
         <v>327</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -6293,7 +6358,7 @@
       <c r="K12" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="L12" s="104" t="s">
+      <c r="L12" s="116" t="s">
         <v>397</v>
       </c>
       <c r="M12" s="21"/>
@@ -6308,17 +6373,17 @@
       <c r="B13" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="102"/>
-      <c r="E13" s="47" t="s">
+      <c r="D13" s="114"/>
+      <c r="E13" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="102" t="s">
+      <c r="F13" s="114" t="s">
         <v>329</v>
       </c>
-      <c r="G13" s="103" t="s">
+      <c r="G13" s="115" t="s">
         <v>400</v>
       </c>
       <c r="H13" s="15"/>
@@ -6326,7 +6391,7 @@
       <c r="K13" s="13">
         <v>0.0</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="49">
         <v>266.0</v>
       </c>
       <c r="M13" s="21"/>
@@ -6341,14 +6406,14 @@
       <c r="B14" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="99"/>
-      <c r="E14" s="47" t="s">
+      <c r="D14" s="110"/>
+      <c r="E14" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="99" t="s">
+      <c r="F14" s="110" t="s">
         <v>330</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -6359,7 +6424,7 @@
       <c r="K14" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="L14" s="104" t="s">
+      <c r="L14" s="116" t="s">
         <v>403</v>
       </c>
       <c r="M14" s="21"/>
@@ -6374,10 +6439,10 @@
       <c r="B15" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F15" s="2" t="s">
@@ -6389,7 +6454,7 @@
       <c r="K15" s="2">
         <v>0.0</v>
       </c>
-      <c r="L15" s="105">
+      <c r="L15" s="117">
         <v>261.0</v>
       </c>
     </row>
@@ -6400,16 +6465,16 @@
       <c r="B16" s="17" t="s">
         <v>408</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="106" t="s">
+      <c r="F16" s="118" t="s">
         <v>320</v>
       </c>
-      <c r="G16" s="94" t="s">
+      <c r="G16" s="105" t="s">
         <v>409</v>
       </c>
       <c r="H16" s="17"/>
@@ -6428,16 +6493,16 @@
       <c r="B17" s="17" t="s">
         <v>411</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E17" s="47" t="s">
+      <c r="E17" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="107" t="s">
+      <c r="F17" s="119" t="s">
         <v>321</v>
       </c>
-      <c r="G17" s="108" t="s">
+      <c r="G17" s="120" t="s">
         <v>412</v>
       </c>
       <c r="H17" s="17"/>
@@ -6445,7 +6510,7 @@
       <c r="K17" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="L17" s="56" t="s">
+      <c r="L17" s="64" t="s">
         <v>414</v>
       </c>
     </row>
@@ -6456,10 +6521,10 @@
       <c r="B18" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="C18" s="109" t="s">
+      <c r="C18" s="121" t="s">
         <v>382</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="55" t="s">
         <v>121</v>
       </c>
       <c r="F18" s="17" t="s">
@@ -6488,10 +6553,10 @@
       <c r="B19" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="C19" s="121" t="s">
         <v>386</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F19" s="17" t="s">
@@ -6520,16 +6585,16 @@
       <c r="B20" s="15" t="s">
         <v>426</v>
       </c>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="55" t="s">
         <v>121</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="G20" s="71" t="s">
+      <c r="G20" s="122" t="s">
         <v>427</v>
       </c>
       <c r="H20" s="15"/>
@@ -6552,16 +6617,16 @@
       <c r="B21" s="15" t="s">
         <v>429</v>
       </c>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="G21" s="71" t="s">
+      <c r="G21" s="79" t="s">
         <v>430</v>
       </c>
       <c r="H21" s="15"/>
@@ -6584,16 +6649,16 @@
       <c r="B22" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="106" t="s">
         <v>382</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="55" t="s">
         <v>121</v>
       </c>
       <c r="F22" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="122" t="s">
         <v>435</v>
       </c>
       <c r="H22" s="15"/>
@@ -6616,16 +6681,16 @@
       <c r="B23" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F23" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="G23" s="71" t="s">
+      <c r="G23" s="79" t="s">
         <v>438</v>
       </c>
       <c r="H23" s="15"/>
@@ -6648,13 +6713,13 @@
       <c r="B24" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="71" t="s">
+      <c r="F24" s="79" t="s">
         <v>438</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -6663,7 +6728,7 @@
       <c r="K24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="110">
+      <c r="L24" s="123">
         <v>242243.0</v>
       </c>
     </row>
@@ -6674,10 +6739,10 @@
       <c r="B25" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F25" s="2" t="s">
@@ -6689,7 +6754,7 @@
       <c r="K25" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L25" s="110" t="s">
+      <c r="L25" s="123" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6700,10 +6765,10 @@
       <c r="B26" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="55" t="s">
         <v>115</v>
       </c>
       <c r="F26" s="2" t="s">
@@ -6715,7 +6780,7 @@
       <c r="K26" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L26" s="110" t="s">
+      <c r="L26" s="123" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6726,22 +6791,22 @@
       <c r="B27" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C27" s="95" t="s">
+      <c r="C27" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E27" s="47" t="s">
+      <c r="E27" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="71" t="s">
+      <c r="F27" s="79" t="s">
         <v>438</v>
       </c>
-      <c r="G27" s="71" t="s">
+      <c r="G27" s="79" t="s">
         <v>455</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L27" s="110" t="s">
+      <c r="L27" s="123" t="s">
         <v>456</v>
       </c>
     </row>
@@ -6752,22 +6817,22 @@
       <c r="B28" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C28" s="95" t="s">
+      <c r="C28" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="E28" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="71" t="s">
+      <c r="F28" s="79" t="s">
         <v>455</v>
       </c>
-      <c r="G28" s="71" t="s">
+      <c r="G28" s="79" t="s">
         <v>459</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L28" s="111">
+      <c r="L28" s="124">
         <v>244221.0</v>
       </c>
     </row>
@@ -6778,75 +6843,75 @@
       <c r="B29" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="106" t="s">
         <v>386</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="71" t="s">
+      <c r="F29" s="79" t="s">
         <v>455</v>
       </c>
-      <c r="G29" s="71" t="s">
+      <c r="G29" s="79" t="s">
         <v>462</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L29" s="112" t="s">
+      <c r="L29" s="125" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="72" t="s">
+      <c r="A30" s="80" t="s">
         <v>464</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="95"/>
+      <c r="C30" s="106"/>
       <c r="D30" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="E30" s="47"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="112"/>
-      <c r="N30" s="113" t="s">
+      <c r="L30" s="125"/>
+      <c r="N30" s="126" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="113" t="s">
+      <c r="A31" s="126" t="s">
         <v>467</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="95"/>
+      <c r="C31" s="106"/>
       <c r="D31" s="2" t="s">
         <v>468</v>
       </c>
-      <c r="E31" s="47"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="79"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="112"/>
+      <c r="L31" s="125"/>
       <c r="N31" s="2" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="113" t="s">
+      <c r="A32" s="126" t="s">
         <v>470</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="95"/>
-      <c r="D32" s="113" t="s">
+      <c r="C32" s="106"/>
+      <c r="D32" s="126" t="s">
         <v>471</v>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
+      <c r="E32" s="55"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="79"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="112"/>
+      <c r="L32" s="125"/>
       <c r="N32" s="2" t="s">
         <v>472</v>
       </c>
@@ -6870,16 +6935,16 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="90" t="s">
         <v>473</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -6887,7 +6952,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="125" t="s">
         <v>365</v>
       </c>
       <c r="D2" s="21"/>
@@ -6921,16 +6986,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="127" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="127" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="127" t="s">
         <v>475</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -6939,7 +7004,7 @@
       <c r="F1" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="127" t="s">
         <v>317</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -6953,9 +7018,9 @@
       <c r="B2" s="25" t="s">
         <v>478</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="116"/>
-      <c r="G2" s="116"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="129"/>
+      <c r="G2" s="129"/>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
@@ -6964,9 +7029,9 @@
       <c r="B3" s="25" t="s">
         <v>479</v>
       </c>
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="G3" s="116"/>
+      <c r="C3" s="129"/>
+      <c r="D3" s="130"/>
+      <c r="G3" s="129"/>
     </row>
     <row r="4" ht="137.25" customHeight="1">
       <c r="A4" s="17" t="s">
@@ -6975,10 +7040,10 @@
       <c r="B4" s="25" t="s">
         <v>480</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="129"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="118"/>
-      <c r="G4" s="117"/>
+      <c r="E4" s="131"/>
+      <c r="G4" s="130"/>
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
@@ -6987,11 +7052,11 @@
       <c r="B5" s="25" t="s">
         <v>481</v>
       </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="117"/>
-      <c r="E5" s="117"/>
-      <c r="F5" s="117"/>
-      <c r="G5" s="117"/>
+      <c r="C5" s="129"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
     </row>
     <row r="6" ht="120.75" customHeight="1">
       <c r="A6" s="17" t="s">
@@ -7000,9 +7065,9 @@
       <c r="B6" s="25" t="s">
         <v>482</v>
       </c>
-      <c r="D6" s="119"/>
-      <c r="E6" s="120"/>
-      <c r="G6" s="116"/>
+      <c r="D6" s="132"/>
+      <c r="E6" s="133"/>
+      <c r="G6" s="129"/>
     </row>
     <row r="7" ht="120.75" customHeight="1">
       <c r="A7" s="17" t="s">
@@ -7011,9 +7076,9 @@
       <c r="B7" s="25" t="s">
         <v>483</v>
       </c>
-      <c r="D7" s="119"/>
-      <c r="E7" s="120"/>
-      <c r="G7" s="116"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="133"/>
+      <c r="G7" s="129"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -7069,7 +7134,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="134" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -7083,20 +7148,20 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="122"/>
-      <c r="C2" s="123"/>
+      <c r="A2" s="135"/>
+      <c r="C2" s="136"/>
     </row>
     <row r="3">
-      <c r="A3" s="124"/>
-      <c r="C3" s="123"/>
+      <c r="A3" s="137"/>
+      <c r="C3" s="136"/>
     </row>
     <row r="4">
-      <c r="A4" s="125"/>
-      <c r="C4" s="123"/>
+      <c r="A4" s="138"/>
+      <c r="C4" s="136"/>
     </row>
     <row r="5">
-      <c r="A5" s="125"/>
-      <c r="C5" s="123"/>
+      <c r="A5" s="138"/>
+      <c r="C5" s="136"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update models, major schema change
publications -> references
external -> ontologyTerms
Publication -> Reference
External -> OntologyTerm

This will affect queries in the absense of additions to a core rdf/owl
schema that adds the requistie subPropertyOf axioms (and some tweaks to
the cypher queries to traverse all subproperties)
</commit_message>
<xml_diff>
--- a/models/dev-layout-conn/source/dev-layout-conn.xlsx
+++ b/models/dev-layout-conn/source/dev-layout-conn.xlsx
@@ -11,7 +11,7 @@
     <sheet state="visible" name="nodes" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="groups" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="neurons" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="publications" sheetId="9" r:id="rId12"/>
+    <sheet state="visible" name="references" sheetId="9" r:id="rId12"/>
     <sheet state="visible" name="localConventions" sheetId="10" r:id="rId13"/>
   </sheets>
   <definedNames/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="516">
   <si>
     <t>id</t>
   </si>
@@ -70,7 +70,7 @@
     <t>Connectivity model used as a reference for developing and testing new layout and visualization code. Based on a simplified version of the bolser lewis model.</t>
   </si>
   <si>
-    <t>external</t>
+    <t>ontologyTerms</t>
   </si>
   <si>
     <t>subtypes</t>
@@ -487,7 +487,7 @@
     <t>NCIT:C41439</t>
   </si>
   <si>
-    <t>External carotid nerve</t>
+    <t>ontologyTerms carotid nerve</t>
   </si>
   <si>
     <t>FMA:6579</t>
@@ -553,7 +553,7 @@
     <t>UBERON:0011326,ILX:0731053</t>
   </si>
   <si>
-    <t>External branch of superior laryngeal nerve</t>
+    <t>ontologyTerms branch of superior laryngeal nerve</t>
   </si>
   <si>
     <t>FMA:6243</t>
@@ -571,7 +571,7 @@
     <t>UBERON:0003716</t>
   </si>
   <si>
-    <t>External branch of inferior laryngeal nerve</t>
+    <t>ontologyTerms branch of inferior laryngeal nerve</t>
   </si>
   <si>
     <t>ILX:0738308</t>
@@ -1003,7 +1003,7 @@
     <t>conveyingLyph</t>
   </si>
   <si>
-    <t>publications</t>
+    <t>references</t>
   </si>
   <si>
     <t>wiredTo</t>
@@ -1129,7 +1129,7 @@
     <t>brain-regions</t>
   </si>
   <si>
-    <t>200, 203, 201</t>
+    <t>200, 203, 204</t>
   </si>
   <si>
     <t>root-2</t>
@@ -1474,7 +1474,13 @@
     <t>layout</t>
   </si>
   <si>
+    <t>anchoredTo</t>
+  </si>
+  <si>
     <t>fixed</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
   <si>
     <t>links</t>
@@ -1598,7 +1604,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="31">
+  <fonts count="28">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1634,17 +1640,13 @@
     </font>
     <font>
       <strike/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <strike/>
       <color rgb="FF555555"/>
       <name val="&quot;Helvetica Neue&quot;"/>
-    </font>
-    <font>
-      <strike/>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF000000"/>
@@ -1666,9 +1668,6 @@
     <font>
       <color rgb="FF555555"/>
       <name val="&quot;docs-Helvetica Neue&quot;"/>
-    </font>
-    <font>
-      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF222222"/>
@@ -1694,7 +1693,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <b/>
       <sz val="9.0"/>
@@ -1821,7 +1819,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1835,6 +1833,9 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1843,9 +1844,6 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1948,7 +1946,7 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1967,7 +1965,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1988,45 +1986,48 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2036,42 +2037,36 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="8" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -2081,13 +2076,13 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2099,7 +2094,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2111,7 +2106,7 @@
     <xf borderId="0" fillId="7" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2123,7 +2118,7 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2132,13 +2127,13 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -2153,100 +2148,113 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="5" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="10" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2548,98 +2556,98 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>492</v>
-      </c>
-      <c r="B2" s="139" t="s">
-        <v>493</v>
+        <v>494</v>
+      </c>
+      <c r="B2" s="143" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>494</v>
-      </c>
-      <c r="B3" s="140" t="s">
-        <v>495</v>
+        <v>496</v>
+      </c>
+      <c r="B3" s="144" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="B4" s="141" t="s">
-        <v>497</v>
+        <v>498</v>
+      </c>
+      <c r="B4" s="145" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>498</v>
-      </c>
-      <c r="B5" s="141" t="s">
-        <v>499</v>
+        <v>500</v>
+      </c>
+      <c r="B5" s="145" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>500</v>
-      </c>
-      <c r="B6" s="141" t="s">
-        <v>501</v>
+        <v>502</v>
+      </c>
+      <c r="B6" s="145" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>502</v>
-      </c>
-      <c r="B7" s="141" t="s">
-        <v>503</v>
+        <v>504</v>
+      </c>
+      <c r="B7" s="145" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>504</v>
-      </c>
-      <c r="B8" s="141" t="s">
-        <v>505</v>
+        <v>506</v>
+      </c>
+      <c r="B8" s="145" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>506</v>
-      </c>
-      <c r="B9" s="141" t="s">
-        <v>507</v>
+        <v>508</v>
+      </c>
+      <c r="B9" s="145" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>508</v>
-      </c>
-      <c r="B10" s="141" t="s">
-        <v>509</v>
+        <v>510</v>
+      </c>
+      <c r="B10" s="145" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>510</v>
-      </c>
-      <c r="B11" s="141" t="s">
-        <v>511</v>
+        <v>512</v>
+      </c>
+      <c r="B11" s="145" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>512</v>
-      </c>
-      <c r="B12" s="142" t="s">
-        <v>513</v>
+        <v>514</v>
+      </c>
+      <c r="B12" s="146" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -2697,37 +2705,37 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="N1" s="8" t="s">
@@ -4042,7 +4050,7 @@
       <c r="A49" s="14">
         <v>235.0</v>
       </c>
-      <c r="B49" s="60" t="s">
+      <c r="B49" s="64" t="s">
         <v>145</v>
       </c>
       <c r="C49" s="53" t="s">
@@ -4233,7 +4241,7 @@
       <c r="T55" s="17"/>
     </row>
     <row r="56">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="65" t="s">
         <v>159</v>
       </c>
       <c r="B56" s="12" t="s">
@@ -4263,7 +4271,7 @@
       <c r="T56" s="17"/>
     </row>
     <row r="57">
-      <c r="A57" s="64" t="s">
+      <c r="A57" s="65" t="s">
         <v>162</v>
       </c>
       <c r="B57" s="12" t="s">
@@ -4281,7 +4289,7 @@
         <v>112.0</v>
       </c>
       <c r="L57" s="15"/>
-      <c r="M57" s="65"/>
+      <c r="M57" s="66"/>
       <c r="N57" s="15"/>
       <c r="O57" s="17"/>
       <c r="P57" s="17"/>
@@ -4290,7 +4298,7 @@
       <c r="T57" s="17"/>
     </row>
     <row r="58">
-      <c r="A58" s="66">
+      <c r="A58" s="67">
         <v>242.0</v>
       </c>
       <c r="B58" s="60" t="s">
@@ -4317,10 +4325,10 @@
       <c r="T58" s="17"/>
     </row>
     <row r="59">
-      <c r="A59" s="66">
+      <c r="A59" s="67">
         <v>243.0</v>
       </c>
-      <c r="B59" s="60" t="s">
+      <c r="B59" s="64" t="s">
         <v>167</v>
       </c>
       <c r="C59" s="24" t="s">
@@ -4344,7 +4352,7 @@
       <c r="T59" s="21"/>
     </row>
     <row r="60">
-      <c r="A60" s="66">
+      <c r="A60" s="67">
         <v>244.0</v>
       </c>
       <c r="B60" s="60" t="s">
@@ -4369,7 +4377,7 @@
       <c r="T60" s="21"/>
     </row>
     <row r="61">
-      <c r="A61" s="67">
+      <c r="A61" s="68">
         <v>245.0</v>
       </c>
       <c r="B61" s="60" t="s">
@@ -4394,13 +4402,13 @@
       <c r="T61" s="21"/>
     </row>
     <row r="62">
-      <c r="A62" s="67">
+      <c r="A62" s="68">
         <v>246.0</v>
       </c>
-      <c r="B62" s="60" t="s">
+      <c r="B62" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="68" t="s">
+      <c r="C62" s="69" t="s">
         <v>174</v>
       </c>
       <c r="D62" s="17"/>
@@ -4419,13 +4427,13 @@
       <c r="T62" s="21"/>
     </row>
     <row r="63">
-      <c r="A63" s="67">
+      <c r="A63" s="68">
         <v>247.0</v>
       </c>
       <c r="B63" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="C63" s="68" t="s">
+      <c r="C63" s="69" t="s">
         <v>176</v>
       </c>
       <c r="D63" s="17"/>
@@ -4444,13 +4452,13 @@
       <c r="T63" s="21"/>
     </row>
     <row r="64">
-      <c r="A64" s="67">
+      <c r="A64" s="68">
         <v>248.0</v>
       </c>
       <c r="B64" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="C64" s="68" t="s">
+      <c r="C64" s="69" t="s">
         <v>178</v>
       </c>
       <c r="D64" s="17"/>
@@ -4459,7 +4467,7 @@
       <c r="G64" s="17"/>
       <c r="I64" s="19"/>
       <c r="J64" s="15"/>
-      <c r="L64" s="69"/>
+      <c r="L64" s="70"/>
       <c r="M64" s="17"/>
       <c r="N64" s="17"/>
       <c r="O64" s="17"/>
@@ -4469,13 +4477,13 @@
       <c r="T64" s="21"/>
     </row>
     <row r="65">
-      <c r="A65" s="67">
+      <c r="A65" s="68">
         <v>249.0</v>
       </c>
       <c r="B65" s="60" t="s">
         <v>179</v>
       </c>
-      <c r="C65" s="68" t="s">
+      <c r="C65" s="69" t="s">
         <v>180</v>
       </c>
       <c r="D65" s="17"/>
@@ -4483,8 +4491,8 @@
       <c r="F65" s="15"/>
       <c r="G65" s="17"/>
       <c r="I65" s="19"/>
-      <c r="J65" s="70"/>
-      <c r="M65" s="71" t="s">
+      <c r="J65" s="71"/>
+      <c r="M65" s="72" t="s">
         <v>181</v>
       </c>
       <c r="N65" s="25">
@@ -4497,13 +4505,13 @@
       <c r="T65" s="21"/>
     </row>
     <row r="66">
-      <c r="A66" s="67">
+      <c r="A66" s="68">
         <v>250.0</v>
       </c>
       <c r="B66" s="60" t="s">
         <v>182</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="69" t="s">
         <v>183</v>
       </c>
       <c r="D66" s="17"/>
@@ -4522,13 +4530,13 @@
       <c r="T66" s="21"/>
     </row>
     <row r="67">
-      <c r="A67" s="67">
+      <c r="A67" s="68">
         <v>251.0</v>
       </c>
       <c r="B67" s="60" t="s">
         <v>184</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="69" t="s">
         <v>185</v>
       </c>
       <c r="D67" s="17"/>
@@ -4547,13 +4555,13 @@
       <c r="T67" s="21"/>
     </row>
     <row r="68">
-      <c r="A68" s="67">
+      <c r="A68" s="68">
         <v>252.0</v>
       </c>
       <c r="B68" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="69" t="s">
         <v>187</v>
       </c>
       <c r="D68" s="17"/>
@@ -4572,13 +4580,13 @@
       <c r="T68" s="21"/>
     </row>
     <row r="69">
-      <c r="A69" s="67">
+      <c r="A69" s="68">
         <v>253.0</v>
       </c>
       <c r="B69" s="60" t="s">
         <v>188</v>
       </c>
-      <c r="C69" s="68" t="s">
+      <c r="C69" s="69" t="s">
         <v>189</v>
       </c>
       <c r="D69" s="17"/>
@@ -4597,13 +4605,13 @@
       <c r="T69" s="21"/>
     </row>
     <row r="70">
-      <c r="A70" s="67">
+      <c r="A70" s="68">
         <v>254.0</v>
       </c>
       <c r="B70" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C70" s="68" t="s">
+      <c r="C70" s="69" t="s">
         <v>191</v>
       </c>
       <c r="D70" s="17"/>
@@ -4622,13 +4630,13 @@
       <c r="T70" s="21"/>
     </row>
     <row r="71">
-      <c r="A71" s="67">
+      <c r="A71" s="68">
         <v>255.0</v>
       </c>
       <c r="B71" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C71" s="72" t="s">
+      <c r="C71" s="73" t="s">
         <v>193</v>
       </c>
       <c r="D71" s="17"/>
@@ -4647,7 +4655,7 @@
       <c r="T71" s="21"/>
     </row>
     <row r="72">
-      <c r="A72" s="67">
+      <c r="A72" s="68">
         <v>256.0</v>
       </c>
       <c r="B72" s="12" t="s">
@@ -4672,13 +4680,13 @@
       <c r="T72" s="21"/>
     </row>
     <row r="73">
-      <c r="A73" s="67">
+      <c r="A73" s="68">
         <v>257.0</v>
       </c>
       <c r="B73" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C73" s="68" t="s">
+      <c r="C73" s="69" t="s">
         <v>197</v>
       </c>
       <c r="D73" s="17"/>
@@ -4697,13 +4705,13 @@
       <c r="T73" s="21"/>
     </row>
     <row r="74">
-      <c r="A74" s="67">
+      <c r="A74" s="68">
         <v>258.0</v>
       </c>
       <c r="B74" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C74" s="68" t="s">
+      <c r="C74" s="69" t="s">
         <v>199</v>
       </c>
       <c r="D74" s="17"/>
@@ -4722,13 +4730,13 @@
       <c r="T74" s="21"/>
     </row>
     <row r="75">
-      <c r="A75" s="67">
+      <c r="A75" s="68">
         <v>259.0</v>
       </c>
       <c r="B75" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C75" s="73" t="s">
+      <c r="C75" s="74" t="s">
         <v>201</v>
       </c>
       <c r="D75" s="17"/>
@@ -4747,10 +4755,10 @@
       <c r="T75" s="21"/>
     </row>
     <row r="76">
-      <c r="A76" s="67">
+      <c r="A76" s="68">
         <v>260.0</v>
       </c>
-      <c r="B76" s="74" t="s">
+      <c r="B76" s="75" t="s">
         <v>202</v>
       </c>
       <c r="C76" s="24" t="s">
@@ -4769,14 +4777,14 @@
       <c r="P76" s="20"/>
       <c r="Q76" s="17"/>
       <c r="R76" s="21"/>
-      <c r="S76" s="75"/>
+      <c r="S76" s="76"/>
       <c r="T76" s="21"/>
     </row>
     <row r="77">
-      <c r="A77" s="67">
+      <c r="A77" s="68">
         <v>261.0</v>
       </c>
-      <c r="B77" s="74" t="s">
+      <c r="B77" s="75" t="s">
         <v>204</v>
       </c>
       <c r="C77" s="16" t="s">
@@ -4795,17 +4803,17 @@
       <c r="P77" s="20"/>
       <c r="Q77" s="17"/>
       <c r="R77" s="21"/>
-      <c r="S77" s="75"/>
+      <c r="S77" s="76"/>
       <c r="T77" s="21"/>
     </row>
     <row r="78">
-      <c r="A78" s="76" t="s">
+      <c r="A78" s="77" t="s">
         <v>206</v>
       </c>
       <c r="B78" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C78" s="68" t="s">
+      <c r="C78" s="69" t="s">
         <v>208</v>
       </c>
       <c r="D78" s="17"/>
@@ -4829,13 +4837,13 @@
       <c r="T78" s="21"/>
     </row>
     <row r="79">
-      <c r="A79" s="76" t="s">
+      <c r="A79" s="77" t="s">
         <v>211</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C79" s="68" t="s">
+      <c r="C79" s="69" t="s">
         <v>213</v>
       </c>
       <c r="D79" s="17"/>
@@ -4859,13 +4867,13 @@
       <c r="T79" s="21"/>
     </row>
     <row r="80">
-      <c r="A80" s="76" t="s">
+      <c r="A80" s="77" t="s">
         <v>214</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C80" s="68" t="s">
+      <c r="C80" s="69" t="s">
         <v>216</v>
       </c>
       <c r="D80" s="17"/>
@@ -4889,13 +4897,13 @@
       <c r="T80" s="21"/>
     </row>
     <row r="81">
-      <c r="A81" s="67">
+      <c r="A81" s="68">
         <v>262.0</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="C81" s="68" t="s">
+      <c r="C81" s="69" t="s">
         <v>218</v>
       </c>
       <c r="D81" s="17"/>
@@ -4915,13 +4923,13 @@
       <c r="T81" s="21"/>
     </row>
     <row r="82">
-      <c r="A82" s="67">
+      <c r="A82" s="68">
         <v>263.0</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="C82" s="68" t="s">
+      <c r="C82" s="69" t="s">
         <v>220</v>
       </c>
       <c r="D82" s="17"/>
@@ -4941,13 +4949,13 @@
       <c r="T82" s="21"/>
     </row>
     <row r="83">
-      <c r="A83" s="67">
+      <c r="A83" s="68">
         <v>264.0</v>
       </c>
       <c r="B83" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C83" s="68" t="s">
+      <c r="C83" s="69" t="s">
         <v>222</v>
       </c>
       <c r="D83" s="17"/>
@@ -4967,13 +4975,13 @@
       <c r="T83" s="21"/>
     </row>
     <row r="84">
-      <c r="A84" s="67">
+      <c r="A84" s="68">
         <v>265.0</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="C84" s="68" t="s">
+      <c r="C84" s="69" t="s">
         <v>224</v>
       </c>
       <c r="D84" s="17"/>
@@ -4982,7 +4990,7 @@
       <c r="G84" s="17"/>
       <c r="I84" s="19"/>
       <c r="J84" s="15"/>
-      <c r="K84" s="77"/>
+      <c r="K84" s="78"/>
       <c r="M84" s="26" t="s">
         <v>225</v>
       </c>
@@ -4996,13 +5004,13 @@
       <c r="T84" s="21"/>
     </row>
     <row r="85">
-      <c r="A85" s="67">
+      <c r="A85" s="68">
         <v>266.0</v>
       </c>
       <c r="B85" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="C85" s="68" t="s">
+      <c r="C85" s="69" t="s">
         <v>227</v>
       </c>
       <c r="D85" s="17"/>
@@ -5011,7 +5019,7 @@
       <c r="G85" s="17"/>
       <c r="I85" s="19"/>
       <c r="J85" s="15"/>
-      <c r="K85" s="77"/>
+      <c r="K85" s="78"/>
       <c r="M85" s="26" t="s">
         <v>228</v>
       </c>
@@ -5025,13 +5033,13 @@
       <c r="T85" s="21"/>
     </row>
     <row r="86">
-      <c r="A86" s="76" t="s">
+      <c r="A86" s="77" t="s">
         <v>229</v>
       </c>
       <c r="B86" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="C86" s="68" t="s">
+      <c r="C86" s="69" t="s">
         <v>231</v>
       </c>
       <c r="D86" s="17"/>
@@ -5042,7 +5050,7 @@
       <c r="J86" s="14">
         <v>108.0</v>
       </c>
-      <c r="K86" s="77"/>
+      <c r="K86" s="78"/>
       <c r="M86" s="14">
         <v>257.0</v>
       </c>
@@ -5056,13 +5064,13 @@
       <c r="T86" s="21"/>
     </row>
     <row r="87">
-      <c r="A87" s="76" t="s">
+      <c r="A87" s="77" t="s">
         <v>232</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>233</v>
       </c>
-      <c r="C87" s="68" t="s">
+      <c r="C87" s="69" t="s">
         <v>234</v>
       </c>
       <c r="D87" s="17"/>
@@ -5073,7 +5081,7 @@
       <c r="J87" s="14">
         <v>109.0</v>
       </c>
-      <c r="K87" s="77"/>
+      <c r="K87" s="78"/>
       <c r="L87" s="15"/>
       <c r="M87" s="15"/>
       <c r="N87" s="17"/>
@@ -5090,7 +5098,7 @@
       <c r="B88" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="C88" s="78" t="s">
+      <c r="C88" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D88" s="17"/>
@@ -5101,7 +5109,7 @@
       <c r="J88" s="14">
         <v>229.0</v>
       </c>
-      <c r="K88" s="77"/>
+      <c r="K88" s="78"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15"/>
       <c r="N88" s="17"/>
@@ -5120,7 +5128,7 @@
       <c r="B89" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="C89" s="78" t="s">
+      <c r="C89" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D89" s="17"/>
@@ -5131,7 +5139,7 @@
       <c r="J89" s="14">
         <v>229.0</v>
       </c>
-      <c r="K89" s="77"/>
+      <c r="K89" s="78"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15"/>
       <c r="N89" s="17"/>
@@ -5150,7 +5158,7 @@
       <c r="B90" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="C90" s="78" t="s">
+      <c r="C90" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D90" s="17"/>
@@ -5161,7 +5169,7 @@
       <c r="J90" s="14">
         <v>229.0</v>
       </c>
-      <c r="K90" s="77"/>
+      <c r="K90" s="78"/>
       <c r="L90" s="15"/>
       <c r="M90" s="15"/>
       <c r="N90" s="17"/>
@@ -5180,7 +5188,7 @@
       <c r="B91" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="C91" s="78" t="s">
+      <c r="C91" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D91" s="17"/>
@@ -5210,7 +5218,7 @@
       <c r="B92" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C92" s="78" t="s">
+      <c r="C92" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D92" s="17"/>
@@ -5221,7 +5229,7 @@
       <c r="J92" s="14">
         <v>229.0</v>
       </c>
-      <c r="K92" s="77"/>
+      <c r="K92" s="78"/>
       <c r="L92" s="15"/>
       <c r="M92" s="15"/>
       <c r="N92" s="17"/>
@@ -5241,7 +5249,7 @@
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A93,1),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (4) (bolew)</v>
       </c>
-      <c r="C93" s="78" t="s">
+      <c r="C93" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D93" s="17"/>
@@ -5252,7 +5260,7 @@
       <c r="J93" s="14">
         <v>229.0</v>
       </c>
-      <c r="K93" s="77"/>
+      <c r="K93" s="78"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15"/>
       <c r="N93" s="17"/>
@@ -5272,7 +5280,7 @@
         <f>concat("Soma in superior cervical ganglion (",CONCAT(right(A94,2),") (bolew)"))</f>
         <v>Soma in superior cervical ganglion (10) (bolew)</v>
       </c>
-      <c r="C94" s="78" t="s">
+      <c r="C94" s="79" t="s">
         <v>236</v>
       </c>
       <c r="D94" s="17"/>
@@ -5283,7 +5291,7 @@
       <c r="J94" s="14">
         <v>229.0</v>
       </c>
-      <c r="K94" s="77"/>
+      <c r="K94" s="78"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15"/>
       <c r="N94" s="17"/>
@@ -5296,22 +5304,22 @@
       <c r="T94" s="21"/>
     </row>
     <row r="95">
-      <c r="A95" s="79" t="s">
+      <c r="A95" s="80" t="s">
         <v>249</v>
       </c>
-      <c r="B95" s="80" t="s">
+      <c r="B95" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="C95" s="78"/>
+      <c r="C95" s="79"/>
       <c r="D95" s="17"/>
       <c r="E95" s="18"/>
       <c r="F95" s="15"/>
       <c r="G95" s="17"/>
       <c r="I95" s="19"/>
       <c r="J95" s="14"/>
-      <c r="K95" s="77"/>
-      <c r="M95" s="81"/>
-      <c r="N95" s="81"/>
+      <c r="K95" s="78"/>
+      <c r="M95" s="25"/>
+      <c r="N95" s="25"/>
       <c r="O95" s="17"/>
       <c r="P95" s="17"/>
       <c r="Q95" s="20"/>
@@ -5340,16 +5348,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="81" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="83" t="s">
+      <c r="C1" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="81" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5360,10 +5368,10 @@
       <c r="B2" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="83" t="s">
         <v>252</v>
       </c>
-      <c r="D2" s="85"/>
+      <c r="D2" s="84"/>
     </row>
     <row r="3">
       <c r="A3" s="14">
@@ -5375,7 +5383,7 @@
       <c r="C3" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="D3" s="85"/>
+      <c r="D3" s="84"/>
     </row>
     <row r="4">
       <c r="A4" s="14">
@@ -5384,7 +5392,7 @@
       <c r="B4" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="85" t="s">
         <v>256</v>
       </c>
       <c r="D4" s="48"/>
@@ -5399,7 +5407,7 @@
       <c r="C5" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="86" t="s">
         <v>259</v>
       </c>
     </row>
@@ -5422,7 +5430,7 @@
       <c r="B7" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="C7" s="87" t="s">
         <v>263</v>
       </c>
       <c r="D7" s="17"/>
@@ -5434,7 +5442,7 @@
       <c r="B8" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="87" t="s">
         <v>265</v>
       </c>
       <c r="D8" s="17"/>
@@ -5446,7 +5454,7 @@
       <c r="B9" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="C9" s="88" t="s">
+      <c r="C9" s="87" t="s">
         <v>267</v>
       </c>
       <c r="D9" s="17"/>
@@ -5546,7 +5554,7 @@
       <c r="B17" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="88" t="s">
         <v>283</v>
       </c>
       <c r="D17" s="17"/>
@@ -5799,28 +5807,28 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="89" t="s">
         <v>314</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="89" t="s">
         <v>315</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="89" t="s">
         <v>316</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="89" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="90" t="s">
         <v>318</v>
       </c>
     </row>
@@ -5876,7 +5884,7 @@
       <c r="H4" s="21"/>
     </row>
     <row r="5">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="80" t="s">
         <v>328</v>
       </c>
       <c r="B5" s="15"/>
@@ -5981,49 +5989,49 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="89" t="s">
         <v>340</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="89" t="s">
         <v>341</v>
       </c>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="91" t="s">
         <v>342</v>
       </c>
-      <c r="G1" s="90" t="s">
+      <c r="G1" s="89" t="s">
         <v>343</v>
       </c>
-      <c r="H1" s="90" t="s">
+      <c r="H1" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="89" t="s">
         <v>344</v>
       </c>
-      <c r="J1" s="93" t="s">
+      <c r="J1" s="92" t="s">
         <v>345</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="89" t="s">
         <v>346</v>
       </c>
-      <c r="L1" s="94" t="s">
+      <c r="L1" s="93" t="s">
         <v>347</v>
       </c>
-      <c r="M1" s="91" t="s">
+      <c r="M1" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="N1" s="91" t="s">
+      <c r="N1" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="91" t="s">
+      <c r="O1" s="90" t="s">
         <v>318</v>
       </c>
       <c r="P1" s="13" t="s">
@@ -6031,32 +6039,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="94" t="s">
         <v>349</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98" t="s">
+      <c r="E2" s="96"/>
+      <c r="F2" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="G2" s="99" t="s">
+      <c r="G2" s="98" t="s">
         <v>351</v>
       </c>
-      <c r="H2" s="100"/>
+      <c r="H2" s="99"/>
       <c r="I2" s="45"/>
       <c r="J2" s="45"/>
       <c r="K2" s="45"/>
       <c r="L2" s="45"/>
       <c r="M2" s="45"/>
       <c r="N2" s="45"/>
-      <c r="O2" s="99" t="s">
+      <c r="O2" s="98" t="s">
         <v>352</v>
       </c>
-      <c r="P2" s="99"/>
+      <c r="P2" s="98"/>
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
@@ -6064,17 +6072,17 @@
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="101" t="s">
+      <c r="D3" s="100" t="s">
         <v>354</v>
       </c>
       <c r="E3" s="21"/>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="101" t="s">
         <v>355</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>356</v>
       </c>
-      <c r="H3" s="103"/>
+      <c r="H3" s="102"/>
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
       <c r="K3" s="21"/>
@@ -6097,13 +6105,13 @@
         <v>359</v>
       </c>
       <c r="E4" s="21"/>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="101" t="s">
         <v>360</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="H4" s="103"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
@@ -6114,7 +6122,7 @@
         <v>362</v>
       </c>
       <c r="P4" s="13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -6122,14 +6130,14 @@
         <v>363</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="D5" s="104" t="s">
+      <c r="D5" s="103" t="s">
         <v>364</v>
       </c>
       <c r="E5" s="55"/>
-      <c r="F5" s="105" t="s">
+      <c r="F5" s="104" t="s">
         <v>365</v>
       </c>
-      <c r="G5" s="105" t="s">
+      <c r="G5" s="104" t="s">
         <v>366</v>
       </c>
       <c r="H5" s="15"/>
@@ -6147,15 +6155,15 @@
         <v>367</v>
       </c>
       <c r="B6" s="15"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="107" t="s">
+      <c r="C6" s="105"/>
+      <c r="D6" s="106" t="s">
         <v>368</v>
       </c>
       <c r="E6" s="55"/>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="104" t="s">
         <v>369</v>
       </c>
-      <c r="G6" s="105" t="s">
+      <c r="G6" s="104" t="s">
         <v>370</v>
       </c>
       <c r="H6" s="15"/>
@@ -6165,7 +6173,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="80" t="s">
+      <c r="O6" s="13" t="s">
         <v>371</v>
       </c>
       <c r="P6" s="13" t="b">
@@ -6177,15 +6185,15 @@
         <v>372</v>
       </c>
       <c r="B7" s="15"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="108">
+      <c r="C7" s="105"/>
+      <c r="D7" s="107">
         <v>227.0</v>
       </c>
       <c r="E7" s="55"/>
-      <c r="F7" s="105" t="s">
+      <c r="F7" s="104" t="s">
         <v>373</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="104" t="s">
         <v>374</v>
       </c>
       <c r="H7" s="15"/>
@@ -6195,7 +6203,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="80" t="s">
+      <c r="O7" s="13" t="s">
         <v>375</v>
       </c>
       <c r="P7" s="13" t="b">
@@ -6207,15 +6215,15 @@
         <v>376</v>
       </c>
       <c r="B8" s="15"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="108">
+      <c r="C8" s="105"/>
+      <c r="D8" s="107">
         <v>259.0</v>
       </c>
       <c r="E8" s="55"/>
-      <c r="F8" s="105" t="s">
+      <c r="F8" s="104" t="s">
         <v>377</v>
       </c>
-      <c r="G8" s="105" t="s">
+      <c r="G8" s="104" t="s">
         <v>378</v>
       </c>
       <c r="H8" s="15"/>
@@ -6225,7 +6233,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="80" t="s">
+      <c r="O8" s="13" t="s">
         <v>379</v>
       </c>
       <c r="P8" s="13" t="b">
@@ -6239,17 +6247,17 @@
       <c r="B9" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="C9" s="106" t="s">
+      <c r="C9" s="105" t="s">
         <v>382</v>
       </c>
-      <c r="D9" s="109"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F9" s="110" t="s">
+      <c r="F9" s="109" t="s">
         <v>323</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="104" t="s">
         <v>383</v>
       </c>
       <c r="H9" s="15"/>
@@ -6273,26 +6281,26 @@
       <c r="B10" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="C10" s="106" t="s">
+      <c r="C10" s="105" t="s">
         <v>386</v>
       </c>
-      <c r="D10" s="109"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F10" s="110" t="s">
+      <c r="F10" s="109" t="s">
         <v>324</v>
       </c>
-      <c r="G10" s="111" t="s">
+      <c r="G10" s="110" t="s">
         <v>387</v>
       </c>
       <c r="H10" s="15"/>
-      <c r="I10" s="112"/>
+      <c r="I10" s="111"/>
       <c r="J10" s="17"/>
-      <c r="K10" s="113" t="s">
+      <c r="K10" s="112" t="s">
         <v>388</v>
       </c>
-      <c r="L10" s="112" t="s">
+      <c r="L10" s="111" t="s">
         <v>389</v>
       </c>
       <c r="M10" s="21"/>
@@ -6307,17 +6315,17 @@
       <c r="B11" s="15" t="s">
         <v>391</v>
       </c>
-      <c r="C11" s="106" t="s">
+      <c r="C11" s="105" t="s">
         <v>382</v>
       </c>
-      <c r="D11" s="114"/>
+      <c r="D11" s="113"/>
       <c r="E11" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="114" t="s">
+      <c r="F11" s="113" t="s">
         <v>326</v>
       </c>
-      <c r="G11" s="115" t="s">
+      <c r="G11" s="114" t="s">
         <v>392</v>
       </c>
       <c r="H11" s="15"/>
@@ -6340,14 +6348,14 @@
       <c r="B12" s="15" t="s">
         <v>394</v>
       </c>
-      <c r="C12" s="106" t="s">
+      <c r="C12" s="105" t="s">
         <v>386</v>
       </c>
-      <c r="D12" s="110"/>
+      <c r="D12" s="109"/>
       <c r="E12" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F12" s="110" t="s">
+      <c r="F12" s="109" t="s">
         <v>327</v>
       </c>
       <c r="G12" s="2" t="s">
@@ -6358,7 +6366,7 @@
       <c r="K12" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="L12" s="116" t="s">
+      <c r="L12" s="115" t="s">
         <v>397</v>
       </c>
       <c r="M12" s="21"/>
@@ -6373,17 +6381,17 @@
       <c r="B13" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="105" t="s">
         <v>382</v>
       </c>
-      <c r="D13" s="114"/>
+      <c r="D13" s="113"/>
       <c r="E13" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="114" t="s">
+      <c r="F13" s="113" t="s">
         <v>329</v>
       </c>
-      <c r="G13" s="115" t="s">
+      <c r="G13" s="114" t="s">
         <v>400</v>
       </c>
       <c r="H13" s="15"/>
@@ -6406,14 +6414,14 @@
       <c r="B14" s="15" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="105" t="s">
         <v>386</v>
       </c>
-      <c r="D14" s="110"/>
+      <c r="D14" s="109"/>
       <c r="E14" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F14" s="110" t="s">
+      <c r="F14" s="109" t="s">
         <v>330</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -6424,7 +6432,7 @@
       <c r="K14" s="13" t="s">
         <v>396</v>
       </c>
-      <c r="L14" s="116" t="s">
+      <c r="L14" s="115" t="s">
         <v>403</v>
       </c>
       <c r="M14" s="21"/>
@@ -6439,7 +6447,7 @@
       <c r="B15" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="C15" s="106" t="s">
+      <c r="C15" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E15" s="55" t="s">
@@ -6454,65 +6462,77 @@
       <c r="K15" s="2">
         <v>0.0</v>
       </c>
-      <c r="L15" s="117">
+      <c r="L15" s="116">
         <v>261.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>407</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="C16" s="106" t="s">
+      <c r="C16" s="117" t="s">
         <v>382</v>
       </c>
-      <c r="E16" s="55" t="s">
+      <c r="D16" s="118"/>
+      <c r="E16" s="119" t="s">
         <v>121</v>
       </c>
-      <c r="F16" s="118" t="s">
+      <c r="F16" s="120" t="s">
         <v>320</v>
       </c>
-      <c r="G16" s="105" t="s">
+      <c r="G16" s="121" t="s">
         <v>409</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="2">
+      <c r="H16" s="19"/>
+      <c r="I16" s="118"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="122">
         <v>0.0</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="122">
         <v>202.0</v>
       </c>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
+      <c r="P16" s="118"/>
     </row>
     <row r="17">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>410</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="19" t="s">
         <v>411</v>
       </c>
-      <c r="C17" s="106" t="s">
+      <c r="C17" s="117" t="s">
         <v>386</v>
       </c>
-      <c r="E17" s="55" t="s">
+      <c r="D17" s="118"/>
+      <c r="E17" s="119" t="s">
         <v>115</v>
       </c>
-      <c r="F17" s="119" t="s">
+      <c r="F17" s="123" t="s">
         <v>321</v>
       </c>
-      <c r="G17" s="120" t="s">
+      <c r="G17" s="124" t="s">
         <v>412</v>
       </c>
-      <c r="H17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="2" t="s">
+      <c r="H17" s="19"/>
+      <c r="I17" s="118"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="122" t="s">
         <v>413</v>
       </c>
-      <c r="L17" s="64" t="s">
+      <c r="L17" s="125" t="s">
         <v>414</v>
       </c>
+      <c r="M17" s="118"/>
+      <c r="N17" s="118"/>
+      <c r="O17" s="118"/>
+      <c r="P17" s="118"/>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
@@ -6521,7 +6541,7 @@
       <c r="B18" s="15" t="s">
         <v>416</v>
       </c>
-      <c r="C18" s="121" t="s">
+      <c r="C18" s="126" t="s">
         <v>382</v>
       </c>
       <c r="E18" s="55" t="s">
@@ -6553,7 +6573,7 @@
       <c r="B19" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="C19" s="121" t="s">
+      <c r="C19" s="126" t="s">
         <v>386</v>
       </c>
       <c r="E19" s="55" t="s">
@@ -6585,7 +6605,7 @@
       <c r="B20" s="15" t="s">
         <v>426</v>
       </c>
-      <c r="C20" s="106" t="s">
+      <c r="C20" s="105" t="s">
         <v>382</v>
       </c>
       <c r="E20" s="55" t="s">
@@ -6594,7 +6614,7 @@
       <c r="F20" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="G20" s="122" t="s">
+      <c r="G20" s="127" t="s">
         <v>427</v>
       </c>
       <c r="H20" s="15"/>
@@ -6617,7 +6637,7 @@
       <c r="B21" s="15" t="s">
         <v>429</v>
       </c>
-      <c r="C21" s="106" t="s">
+      <c r="C21" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E21" s="55" t="s">
@@ -6626,7 +6646,7 @@
       <c r="F21" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="G21" s="79" t="s">
+      <c r="G21" s="80" t="s">
         <v>430</v>
       </c>
       <c r="H21" s="15"/>
@@ -6649,7 +6669,7 @@
       <c r="B22" s="15" t="s">
         <v>434</v>
       </c>
-      <c r="C22" s="106" t="s">
+      <c r="C22" s="105" t="s">
         <v>382</v>
       </c>
       <c r="E22" s="55" t="s">
@@ -6658,7 +6678,7 @@
       <c r="F22" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="G22" s="122" t="s">
+      <c r="G22" s="127" t="s">
         <v>435</v>
       </c>
       <c r="H22" s="15"/>
@@ -6681,7 +6701,7 @@
       <c r="B23" s="15" t="s">
         <v>437</v>
       </c>
-      <c r="C23" s="106" t="s">
+      <c r="C23" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E23" s="55" t="s">
@@ -6690,7 +6710,7 @@
       <c r="F23" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="G23" s="79" t="s">
+      <c r="G23" s="80" t="s">
         <v>438</v>
       </c>
       <c r="H23" s="15"/>
@@ -6713,13 +6733,13 @@
       <c r="B24" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="C24" s="106" t="s">
+      <c r="C24" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E24" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="79" t="s">
+      <c r="F24" s="80" t="s">
         <v>438</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -6728,7 +6748,7 @@
       <c r="K24" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L24" s="123">
+      <c r="L24" s="128">
         <v>242243.0</v>
       </c>
     </row>
@@ -6739,7 +6759,7 @@
       <c r="B25" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="C25" s="106" t="s">
+      <c r="C25" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E25" s="55" t="s">
@@ -6754,7 +6774,7 @@
       <c r="K25" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L25" s="123" t="s">
+      <c r="L25" s="128" t="s">
         <v>448</v>
       </c>
     </row>
@@ -6765,7 +6785,7 @@
       <c r="B26" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="C26" s="106" t="s">
+      <c r="C26" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E26" s="55" t="s">
@@ -6780,7 +6800,7 @@
       <c r="K26" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L26" s="123" t="s">
+      <c r="L26" s="128" t="s">
         <v>452</v>
       </c>
     </row>
@@ -6791,22 +6811,22 @@
       <c r="B27" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="C27" s="106" t="s">
+      <c r="C27" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E27" s="55" t="s">
         <v>118</v>
       </c>
-      <c r="F27" s="79" t="s">
+      <c r="F27" s="80" t="s">
         <v>438</v>
       </c>
-      <c r="G27" s="79" t="s">
+      <c r="G27" s="80" t="s">
         <v>455</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="L27" s="123" t="s">
+      <c r="L27" s="128" t="s">
         <v>456</v>
       </c>
     </row>
@@ -6817,22 +6837,22 @@
       <c r="B28" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="C28" s="106" t="s">
+      <c r="C28" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E28" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="79" t="s">
+      <c r="F28" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="G28" s="79" t="s">
+      <c r="G28" s="80" t="s">
         <v>459</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L28" s="124">
+      <c r="L28" s="129">
         <v>244221.0</v>
       </c>
     </row>
@@ -6843,75 +6863,75 @@
       <c r="B29" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="C29" s="106" t="s">
+      <c r="C29" s="105" t="s">
         <v>386</v>
       </c>
       <c r="E29" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="F29" s="79" t="s">
+      <c r="F29" s="80" t="s">
         <v>455</v>
       </c>
-      <c r="G29" s="79" t="s">
+      <c r="G29" s="80" t="s">
         <v>462</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="L29" s="125" t="s">
+      <c r="L29" s="130" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="80" t="s">
+      <c r="A30" s="13" t="s">
         <v>464</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="106"/>
+      <c r="C30" s="105"/>
       <c r="D30" s="2" t="s">
         <v>465</v>
       </c>
       <c r="E30" s="55"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
+      <c r="F30" s="80"/>
+      <c r="G30" s="80"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="125"/>
-      <c r="N30" s="126" t="s">
+      <c r="L30" s="130"/>
+      <c r="N30" s="2" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="126" t="s">
+      <c r="A31" s="2" t="s">
         <v>467</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="106"/>
+      <c r="C31" s="105"/>
       <c r="D31" s="2" t="s">
         <v>468</v>
       </c>
       <c r="E31" s="55"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
       <c r="K31" s="2"/>
-      <c r="L31" s="125"/>
+      <c r="L31" s="130"/>
       <c r="N31" s="2" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="126" t="s">
+      <c r="A32" s="2" t="s">
         <v>470</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="106"/>
-      <c r="D32" s="126" t="s">
+      <c r="C32" s="105"/>
+      <c r="D32" s="2" t="s">
         <v>471</v>
       </c>
       <c r="E32" s="55"/>
-      <c r="F32" s="79"/>
-      <c r="G32" s="79"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="125"/>
+      <c r="L32" s="130"/>
       <c r="N32" s="2" t="s">
         <v>472</v>
       </c>
@@ -6935,27 +6955,33 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="89" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="89" t="s">
         <v>473</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="90" t="s">
         <v>474</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="130" t="s">
         <v>365</v>
       </c>
       <c r="D2" s="21"/>
+      <c r="E2" s="13" t="s">
+        <v>476</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6986,25 +7012,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="127" t="s">
+      <c r="A1" s="131" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="127" t="s">
+      <c r="C1" s="131" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="127" t="s">
-        <v>475</v>
+      <c r="D1" s="131" t="s">
+        <v>477</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="G1" s="127" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1" s="131" t="s">
         <v>317</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -7016,69 +7042,69 @@
         <v>237</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>478</v>
-      </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="129"/>
-      <c r="G2" s="129"/>
+        <v>480</v>
+      </c>
+      <c r="C2" s="132"/>
+      <c r="D2" s="133"/>
+      <c r="G2" s="133"/>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
         <v>239</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>479</v>
-      </c>
-      <c r="C3" s="129"/>
-      <c r="D3" s="130"/>
-      <c r="G3" s="129"/>
+        <v>481</v>
+      </c>
+      <c r="C3" s="133"/>
+      <c r="D3" s="134"/>
+      <c r="G3" s="133"/>
     </row>
     <row r="4" ht="137.25" customHeight="1">
       <c r="A4" s="17" t="s">
         <v>241</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>480</v>
-      </c>
-      <c r="C4" s="129"/>
+        <v>482</v>
+      </c>
+      <c r="C4" s="133"/>
       <c r="D4" s="12"/>
-      <c r="E4" s="131"/>
-      <c r="G4" s="130"/>
+      <c r="E4" s="135"/>
+      <c r="G4" s="134"/>
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
         <v>244</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>481</v>
-      </c>
-      <c r="C5" s="129"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
+        <v>483</v>
+      </c>
+      <c r="C5" s="133"/>
+      <c r="D5" s="134"/>
+      <c r="E5" s="134"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
     </row>
     <row r="6" ht="120.75" customHeight="1">
       <c r="A6" s="17" t="s">
         <v>246</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>482</v>
-      </c>
-      <c r="D6" s="132"/>
-      <c r="E6" s="133"/>
-      <c r="G6" s="129"/>
+        <v>484</v>
+      </c>
+      <c r="D6" s="136"/>
+      <c r="E6" s="137"/>
+      <c r="G6" s="133"/>
     </row>
     <row r="7" ht="120.75" customHeight="1">
       <c r="A7" s="17" t="s">
         <v>248</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>483</v>
-      </c>
-      <c r="D7" s="132"/>
-      <c r="E7" s="133"/>
-      <c r="G7" s="129"/>
+        <v>485</v>
+      </c>
+      <c r="D7" s="136"/>
+      <c r="E7" s="137"/>
+      <c r="G7" s="133"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -7102,16 +7128,16 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
     </row>
   </sheetData>
@@ -7134,34 +7160,34 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="138" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="135"/>
-      <c r="C2" s="136"/>
+      <c r="A2" s="139"/>
+      <c r="C2" s="140"/>
     </row>
     <row r="3">
-      <c r="A3" s="137"/>
-      <c r="C3" s="136"/>
+      <c r="A3" s="141"/>
+      <c r="C3" s="140"/>
     </row>
     <row r="4">
-      <c r="A4" s="138"/>
-      <c r="C4" s="136"/>
+      <c r="A4" s="142"/>
+      <c r="C4" s="140"/>
     </row>
     <row r="5">
-      <c r="A5" s="138"/>
-      <c r="C5" s="136"/>
+      <c r="A5" s="142"/>
+      <c r="C5" s="140"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>